<commit_message>
Mappings -> Match mappings with the changes made to Instalation Profile.
</commit_message>
<xml_diff>
--- a/xlsx/Lists.xlsx
+++ b/xlsx/Lists.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/git/metadata-schema/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF7DB5C8-0506-4B86-A706-8965F41E9739}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DB7EF3E-118E-4E93-9B61-FB63236E7660}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_Languages" sheetId="2" r:id="rId1"/>
     <sheet name="02_Themes" sheetId="3" r:id="rId2"/>
     <sheet name="03_Cultural Context" sheetId="4" r:id="rId3"/>
     <sheet name="04_Social Groups" sheetId="5" r:id="rId4"/>
-    <sheet name="05_Licences" sheetId="6" r:id="rId5"/>
+    <sheet name="05_Rights" sheetId="6" r:id="rId5"/>
     <sheet name="06_Gender" sheetId="7" r:id="rId6"/>
     <sheet name="07_Cultural Sensitivity" sheetId="8" r:id="rId7"/>
     <sheet name="08_Occupations" sheetId="9" r:id="rId8"/>
     <sheet name="09_Project Types" sheetId="10" r:id="rId9"/>
     <sheet name="10_Project Regions" sheetId="11" r:id="rId10"/>
-    <sheet name="11_Rights Statement" sheetId="12" r:id="rId11"/>
-    <sheet name="12_Roles" sheetId="13" r:id="rId12"/>
-    <sheet name="13_Language Labels" sheetId="15" r:id="rId13"/>
-    <sheet name="14_Authority Sources" sheetId="16" r:id="rId14"/>
+    <sheet name="11_Roles" sheetId="13" r:id="rId11"/>
+    <sheet name="12_Language Labels" sheetId="15" r:id="rId12"/>
+    <sheet name="13_Authority Sources" sheetId="16" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="744">
   <si>
     <t>Term ID</t>
   </si>
@@ -1488,60 +1487,24 @@
     <t>Volunteer groups</t>
   </si>
   <si>
-    <t>licence_01</t>
-  </si>
-  <si>
-    <t>CC BY 4.0</t>
-  </si>
-  <si>
     <t>Attribution---This licence lets others distribute, remix, adapt, and build upon your work, even commercially, as long as they credit you for the original creation. This is the most accommodating of licences offered. Recommended for maximum dissemination and use of licenced materials.</t>
   </si>
   <si>
-    <t>licence_02</t>
-  </si>
-  <si>
-    <t>CC BY-SA 4.0</t>
-  </si>
-  <si>
     <t>Attribution-ShareAlike---This licence lets others remix, adapt, and build upon your work even for commercial purposes, as long as they credit you and licence their new creations under the identical terms. This licence is often compared to “copyleft” free and open source software licences. All new works based on yours will carry the same licence, so any derivatives will also allow commercial use. This is the licence used by Wikipedia, and is recommended for materials that would benefit from incorporating content from Wikipedia and similarly licenced projects.</t>
   </si>
   <si>
-    <t>licence_03</t>
-  </si>
-  <si>
-    <t>CC BY-ND 4.0</t>
-  </si>
-  <si>
     <t>Attribution-NoDerivs---This licence lets others reuse the work for any purpose, including commercially; however, it cannot be shared with others in adapted form, and credit must be provided to you.</t>
   </si>
   <si>
-    <t>licence_04</t>
-  </si>
-  <si>
-    <t>CC BY-NC-SA 4.0</t>
-  </si>
-  <si>
     <t>Attribution-NonCommercial-ShareAlike---This licence lets others remix, adapt, and build upon your work non-commercially, as long as they credit you and licence their new creations under the identical terms.</t>
   </si>
   <si>
-    <t>licence_05</t>
-  </si>
-  <si>
-    <t>CC BY-NC-ND 4.0</t>
-  </si>
-  <si>
     <t>Attribution-NonCommercial-NoDerivs---This licence is the most restrictive of our six main licences, only allowing others to download your works and share them with others as long as they credit you, but they can’t change them in any way or use them commercially.</t>
   </si>
   <si>
-    <t>licence_06</t>
-  </si>
-  <si>
     <t>CC0</t>
   </si>
   <si>
-    <t>Public Domain--- is a public dedication tool, which allows creators to give up their copyright and put their works into the worldwide public domain. CC0 allows reusers to distribute, remix, adapt, and build upon the material in any medium or format, with no conditions.</t>
-  </si>
-  <si>
     <t>gender_001</t>
   </si>
   <si>
@@ -2055,108 +2018,72 @@
     <t>North America</t>
   </si>
   <si>
-    <t>rs_001</t>
-  </si>
-  <si>
     <t>In Copyright (InC)</t>
   </si>
   <si>
     <t>indicates that the Item labeled with this Rights Statement is in copyright.</t>
   </si>
   <si>
-    <t>rs_002</t>
-  </si>
-  <si>
     <t>In Copyright - EU Orphan Work (InC-OW-EU)</t>
   </si>
   <si>
     <t>indicates that the Item labeled with this Rights Statement has been identified as an ‘Orphan Work’ under the terms of the EU Orphan Works Directive.</t>
   </si>
   <si>
-    <t>rs_003</t>
-  </si>
-  <si>
     <t>In Copyright - Rights-holder(s) Unlocatable or Unidentifiable (InC-RUU)</t>
   </si>
   <si>
     <t>indicates that the Item labeled with this Rights Statement has been identified as in copyright, but whose rights-holder(s) either cannot be identified or cannot be located.</t>
   </si>
   <si>
-    <t>rs_004</t>
-  </si>
-  <si>
     <t>In Copyright - Educational Use Permitted (InC-EDU)</t>
   </si>
   <si>
     <t>indicates that the Item labeled with this Rights Statement is in copyright but that educational use is allowed without the need to obtain additional permission.</t>
   </si>
   <si>
-    <t>rs_005</t>
-  </si>
-  <si>
     <t>In Copyright - Non-Commercial Use Permitted (InC-NC)</t>
   </si>
   <si>
     <t>indicates that the Item labeled with this Rights Statement is in copyright but that non-commercial use is allowed without the need to obtain additional permission.</t>
   </si>
   <si>
-    <t>rs_006</t>
-  </si>
-  <si>
     <t>No Copyright - Non-Commercial Use Only (NoC-NC)</t>
   </si>
   <si>
     <t>indicates that the underlying Work is in the Public Domain, but the organization that has published the Item is contractually required to allow only non-commercial use by third parties.</t>
   </si>
   <si>
-    <t>rs_007</t>
-  </si>
-  <si>
     <t>No Copyright - Contractual Restrictions (NoC-CR)</t>
   </si>
   <si>
     <t>indicates that the underlying Work is in the Public Domain, but the organization that has published the Item is contractually required to restrict certain forms of use by third parties.</t>
   </si>
   <si>
-    <t>rs_008</t>
-  </si>
-  <si>
     <t>No Copyright - Other Known Legal Restrictions (NoC-OKLR)</t>
   </si>
   <si>
     <t>indicates that the underlying Work is in the Public Domain, but that laws other than copyright impose restrictions on the use of the Item by third parties.</t>
   </si>
   <si>
-    <t>rs_009</t>
-  </si>
-  <si>
     <t>No Copyright - United States (NoC-US)</t>
   </si>
   <si>
     <t>indicates that the underlying Work is in the Public Domain under the laws of the United States, but that a determination was not made as to its copyright status under the copyright laws of other countries.</t>
   </si>
   <si>
-    <t>rs_010</t>
-  </si>
-  <si>
     <t>No Known Copyright (NKC)</t>
   </si>
   <si>
     <t>indicates that the organization that has published the Item believes that no copyright or related rights are known to exist, but that a conclusive determination could not be made.</t>
   </si>
   <si>
-    <t>rs_011</t>
-  </si>
-  <si>
     <t>Copyright Not Evaluated (CNE)</t>
   </si>
   <si>
     <t>indicates that the organization that has published the Item has not evaluated the copyright and related rights status of the Item.</t>
   </si>
   <si>
-    <t>rs_012</t>
-  </si>
-  <si>
     <t>Copyright Undetermined (UND)</t>
   </si>
   <si>
@@ -2263,6 +2190,109 @@
   </si>
   <si>
     <t>MAs Projects</t>
+  </si>
+  <si>
+    <t>Creative Commons - Attribution</t>
+  </si>
+  <si>
+    <t>Creative Commons BY-NC</t>
+  </si>
+  <si>
+    <t>Creative Commons BY-NC-ND</t>
+  </si>
+  <si>
+    <t>Creative Commons BY-NC-SA</t>
+  </si>
+  <si>
+    <t>Creative Commons BY-ND</t>
+  </si>
+  <si>
+    <t>Creative Commons BY-SA</t>
+  </si>
+  <si>
+    <t>Creative Commons 0</t>
+  </si>
+  <si>
+    <t>Public Domain Mark</t>
+  </si>
+  <si>
+    <t>cc_by</t>
+  </si>
+  <si>
+    <t>cc_by_nc</t>
+  </si>
+  <si>
+    <t>cc_by_nc_sa</t>
+  </si>
+  <si>
+    <t>cc_by_nd</t>
+  </si>
+  <si>
+    <t>cc_by_sa</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>inc_edu</t>
+  </si>
+  <si>
+    <t>inc_ow_eu</t>
+  </si>
+  <si>
+    <t>inc_nc</t>
+  </si>
+  <si>
+    <t>inc_ruu</t>
+  </si>
+  <si>
+    <t>noc_cr</t>
+  </si>
+  <si>
+    <t>noc_nc</t>
+  </si>
+  <si>
+    <t>noc_oklr</t>
+  </si>
+  <si>
+    <t>noc_us</t>
+  </si>
+  <si>
+    <t>cne</t>
+  </si>
+  <si>
+    <t>und</t>
+  </si>
+  <si>
+    <t>nkc</t>
+  </si>
+  <si>
+    <t>pdm</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial 4.0 International---This license enables reusers to distribute, remix, adapt, and build upon the material in any medium or format for noncommercial purposes only, and only so long as attribution is given to the creator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cc_by_nc_nd </t>
+  </si>
+  <si>
+    <t>CC0 (“CC Zero”) is intended for use only
+by authors or holders of copyright and
+related rights (including database rights), in connection
+with works that are still subject to those rights in one or
+more countries.
+When CC0 is applied to a work, copyright and related
+rights are relinquished worldwide, making the work free
+from those restrictions to the greatest extent possible.</t>
+  </si>
+  <si>
+    <t>The Public Domain Mark (PDM) is used
+to label works that are already free of
+known copyright restrictions. Unlike CC0, PDM doesn’t
+change the copyright status of a work.
+PDM can be used by anyone, and is intended for use
+with works that are already free of known copyright
+restrictions throughout the world.</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2397,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2378,6 +2408,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4551,50 +4584,50 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>658</v>
+        <v>646</v>
       </c>
       <c r="B3" t="s">
-        <v>659</v>
+        <v>647</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>660</v>
+        <v>648</v>
       </c>
       <c r="B4" t="s">
-        <v>661</v>
+        <v>649</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>662</v>
+        <v>650</v>
       </c>
       <c r="B5" t="s">
-        <v>734</v>
+        <v>710</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>663</v>
+        <v>651</v>
       </c>
       <c r="B6" t="s">
-        <v>735</v>
+        <v>711</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>664</v>
+        <v>652</v>
       </c>
       <c r="B7" t="s">
-        <v>665</v>
+        <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>666</v>
+        <v>654</v>
       </c>
       <c r="B8" t="s">
-        <v>667</v>
+        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -4603,193 +4636,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F6335E-B01C-4EB6-8502-222DDC2744C7}">
-  <dimension ref="A1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>668</v>
-      </c>
-      <c r="B3" t="s">
-        <v>669</v>
-      </c>
-      <c r="C3" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>671</v>
-      </c>
-      <c r="B4" t="s">
-        <v>672</v>
-      </c>
-      <c r="C4" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>674</v>
-      </c>
-      <c r="B5" t="s">
-        <v>675</v>
-      </c>
-      <c r="C5" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>677</v>
-      </c>
-      <c r="B6" t="s">
-        <v>678</v>
-      </c>
-      <c r="C6" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>680</v>
-      </c>
-      <c r="B7" t="s">
-        <v>681</v>
-      </c>
-      <c r="C7" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>683</v>
-      </c>
-      <c r="B8" t="s">
-        <v>684</v>
-      </c>
-      <c r="C8" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>686</v>
-      </c>
-      <c r="B9" t="s">
-        <v>687</v>
-      </c>
-      <c r="C9" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>689</v>
-      </c>
-      <c r="B10" t="s">
-        <v>690</v>
-      </c>
-      <c r="C10" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>692</v>
-      </c>
-      <c r="B11" t="s">
-        <v>693</v>
-      </c>
-      <c r="C11" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>695</v>
-      </c>
-      <c r="B12" t="s">
-        <v>696</v>
-      </c>
-      <c r="C12" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>698</v>
-      </c>
-      <c r="B13" t="s">
-        <v>699</v>
-      </c>
-      <c r="C13" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>701</v>
-      </c>
-      <c r="B14" t="s">
-        <v>702</v>
-      </c>
-      <c r="C14" t="s">
-        <v>703</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F350B9F1-06F7-4E8A-B44A-16E139FB0B1D}">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -4821,58 +4667,58 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>704</v>
+        <v>680</v>
       </c>
       <c r="B2" t="s">
-        <v>705</v>
+        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>706</v>
+        <v>682</v>
       </c>
       <c r="B3" t="s">
-        <v>707</v>
+        <v>683</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>708</v>
+        <v>684</v>
       </c>
       <c r="B4" t="s">
-        <v>709</v>
+        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>710</v>
+        <v>686</v>
       </c>
       <c r="B5" t="s">
-        <v>711</v>
+        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>712</v>
+        <v>688</v>
       </c>
       <c r="B6" t="s">
-        <v>713</v>
+        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>714</v>
+        <v>690</v>
       </c>
       <c r="B7" t="s">
-        <v>715</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>716</v>
+        <v>692</v>
       </c>
       <c r="B8" t="s">
-        <v>717</v>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -4880,7 +4726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5D6CC2-7C88-44F7-8C63-8AD47A42CD2B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -4912,18 +4758,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>720</v>
+        <v>696</v>
       </c>
       <c r="B2" t="s">
-        <v>718</v>
+        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>721</v>
+        <v>697</v>
       </c>
       <c r="B3" t="s">
-        <v>719</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -4932,12 +4778,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9990D756-E521-44BC-87A8-D4E80EBBCAC7}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4964,46 +4810,46 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>724</v>
+        <v>700</v>
       </c>
       <c r="B2" t="s">
-        <v>722</v>
+        <v>698</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>730</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>725</v>
+        <v>701</v>
       </c>
       <c r="B3" t="s">
-        <v>723</v>
+        <v>699</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>733</v>
+        <v>709</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>726</v>
+        <v>702</v>
       </c>
       <c r="B4" t="s">
-        <v>728</v>
+        <v>704</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>731</v>
+        <v>707</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>727</v>
+        <v>703</v>
       </c>
       <c r="B5" t="s">
-        <v>729</v>
+        <v>705</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>732</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -5016,11 +4862,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477AB8E0-193B-4ACE-9281-1EB5DE711D3C}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
@@ -5395,8 +5245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16B73E5-B011-40A2-8AFF-3FBA72B05675}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5706,8 +5556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3BBE258-A0AD-4181-B80C-BA0C0B18114A}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6067,13 +5917,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B29326D-C093-4910-A1C0-5F486B1575C8}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
@@ -6117,69 +5972,235 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>722</v>
+      </c>
+      <c r="B3" t="s">
+        <v>714</v>
+      </c>
+      <c r="C3" t="s">
         <v>479</v>
-      </c>
-      <c r="B3" t="s">
-        <v>480</v>
-      </c>
-      <c r="C3" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>482</v>
+        <v>723</v>
       </c>
       <c r="B4" t="s">
-        <v>483</v>
+        <v>715</v>
       </c>
       <c r="C4" t="s">
-        <v>484</v>
+        <v>740</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>485</v>
+        <v>741</v>
       </c>
       <c r="B5" t="s">
-        <v>486</v>
+        <v>716</v>
       </c>
       <c r="C5" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>488</v>
+        <v>724</v>
       </c>
       <c r="B6" t="s">
-        <v>489</v>
+        <v>717</v>
       </c>
       <c r="C6" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>491</v>
+        <v>725</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>718</v>
       </c>
       <c r="C7" t="s">
-        <v>493</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>494</v>
+        <v>726</v>
       </c>
       <c r="B8" t="s">
-        <v>495</v>
+        <v>719</v>
       </c>
       <c r="C8" t="s">
-        <v>496</v>
-      </c>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>727</v>
+      </c>
+      <c r="B9" t="s">
+        <v>656</v>
+      </c>
+      <c r="C9" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>728</v>
+      </c>
+      <c r="B10" t="s">
+        <v>662</v>
+      </c>
+      <c r="C10" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>729</v>
+      </c>
+      <c r="B11" t="s">
+        <v>658</v>
+      </c>
+      <c r="C11" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>730</v>
+      </c>
+      <c r="B12" t="s">
+        <v>664</v>
+      </c>
+      <c r="C12" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>731</v>
+      </c>
+      <c r="B13" t="s">
+        <v>660</v>
+      </c>
+      <c r="C13" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>732</v>
+      </c>
+      <c r="B14" t="s">
+        <v>668</v>
+      </c>
+      <c r="C14" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>733</v>
+      </c>
+      <c r="B15" t="s">
+        <v>666</v>
+      </c>
+      <c r="C15" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>734</v>
+      </c>
+      <c r="B16" t="s">
+        <v>670</v>
+      </c>
+      <c r="C16" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>735</v>
+      </c>
+      <c r="B17" t="s">
+        <v>672</v>
+      </c>
+      <c r="C17" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>736</v>
+      </c>
+      <c r="B18" t="s">
+        <v>676</v>
+      </c>
+      <c r="C18" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>737</v>
+      </c>
+      <c r="B19" t="s">
+        <v>678</v>
+      </c>
+      <c r="C19" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>738</v>
+      </c>
+      <c r="B20" t="s">
+        <v>674</v>
+      </c>
+      <c r="C20" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>484</v>
+      </c>
+      <c r="B21" t="s">
+        <v>720</v>
+      </c>
+      <c r="C21" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>739</v>
+      </c>
+      <c r="B22" t="s">
+        <v>721</v>
+      </c>
+      <c r="C22" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C26" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6238,35 +6259,35 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="B3" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="B4" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="B5" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="B6" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -6329,35 +6350,35 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
       <c r="B4" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>511</v>
+        <v>499</v>
       </c>
       <c r="B5" t="s">
-        <v>512</v>
+        <v>500</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -6419,549 +6440,549 @@
         <v>5</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="B3" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="B4" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="B5" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="B6" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="B7" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="B8" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>527</v>
+        <v>515</v>
       </c>
       <c r="B9" t="s">
-        <v>528</v>
+        <v>516</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
       <c r="B10" t="s">
-        <v>530</v>
+        <v>518</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>531</v>
+        <v>519</v>
       </c>
       <c r="B11" t="s">
-        <v>532</v>
+        <v>520</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>533</v>
+        <v>521</v>
       </c>
       <c r="B12" t="s">
-        <v>534</v>
+        <v>522</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>535</v>
+        <v>523</v>
       </c>
       <c r="B13" t="s">
-        <v>536</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>537</v>
+        <v>525</v>
       </c>
       <c r="B14" t="s">
-        <v>538</v>
+        <v>526</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>539</v>
+        <v>527</v>
       </c>
       <c r="B15" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>541</v>
+        <v>529</v>
       </c>
       <c r="B16" t="s">
-        <v>542</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="B17" t="s">
-        <v>544</v>
+        <v>532</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>545</v>
+        <v>533</v>
       </c>
       <c r="B18" t="s">
-        <v>546</v>
+        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="B19" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>549</v>
+        <v>537</v>
       </c>
       <c r="B20" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>551</v>
+        <v>539</v>
       </c>
       <c r="B21" t="s">
-        <v>552</v>
+        <v>540</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>553</v>
+        <v>541</v>
       </c>
       <c r="B22" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>555</v>
+        <v>543</v>
       </c>
       <c r="B23" t="s">
-        <v>556</v>
+        <v>544</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>557</v>
+        <v>545</v>
       </c>
       <c r="B24" t="s">
-        <v>558</v>
+        <v>546</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>559</v>
+        <v>547</v>
       </c>
       <c r="B25" t="s">
-        <v>560</v>
+        <v>548</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>561</v>
+        <v>549</v>
       </c>
       <c r="B26" t="s">
-        <v>562</v>
+        <v>550</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>563</v>
+        <v>551</v>
       </c>
       <c r="B27" t="s">
-        <v>564</v>
+        <v>552</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>565</v>
+        <v>553</v>
       </c>
       <c r="B28" t="s">
-        <v>566</v>
+        <v>554</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>567</v>
+        <v>555</v>
       </c>
       <c r="B29" t="s">
-        <v>568</v>
+        <v>556</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>569</v>
+        <v>557</v>
       </c>
       <c r="B30" t="s">
-        <v>570</v>
+        <v>558</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>571</v>
+        <v>559</v>
       </c>
       <c r="B31" t="s">
-        <v>572</v>
+        <v>560</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>573</v>
+        <v>561</v>
       </c>
       <c r="B32" t="s">
-        <v>574</v>
+        <v>562</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>575</v>
+        <v>563</v>
       </c>
       <c r="B33" t="s">
-        <v>576</v>
+        <v>564</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
       <c r="B34" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>579</v>
+        <v>567</v>
       </c>
       <c r="B35" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="B36" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="B37" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="B38" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="B39" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="B40" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="B41" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="B42" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="B43" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="B44" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="B45" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="B46" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="B47" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="B48" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="B49" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="B50" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="B51" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>613</v>
+        <v>601</v>
       </c>
       <c r="B52" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
       <c r="B53" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="B54" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="B55" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="B56" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="B57" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
       <c r="B58" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="B59" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="B60" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="B61" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="B62" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="B63" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="B64" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="B65" t="s">
-        <v>640</v>
+        <v>628</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="B66" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>643</v>
+        <v>631</v>
       </c>
       <c r="B67" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="B68" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
       <c r="C68" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>648</v>
+        <v>636</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>649</v>
+        <v>637</v>
       </c>
       <c r="C69" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -6974,7 +6995,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J1" sqref="J1:J299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7024,42 +7045,42 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>650</v>
+        <v>638</v>
       </c>
       <c r="B3" t="s">
-        <v>651</v>
+        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>652</v>
+        <v>640</v>
       </c>
       <c r="B4" t="s">
-        <v>653</v>
+        <v>641</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>654</v>
+        <v>642</v>
       </c>
       <c r="B5" t="s">
-        <v>655</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>656</v>
+        <v>644</v>
       </c>
       <c r="B6" t="s">
-        <v>657</v>
+        <v>645</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>736</v>
+        <v>712</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>737</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
traditional knowledge and biocultural labels
</commit_message>
<xml_diff>
--- a/xlsx/Lists.xlsx
+++ b/xlsx/Lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DB7EF3E-118E-4E93-9B61-FB63236E7660}"/>
+  <xr:revisionPtr revIDLastSave="400" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{168892A6-3CCB-41DC-9029-19331CF7CDF7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1875" yWindow="900" windowWidth="11220" windowHeight="16605" firstSheet="14" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_Languages" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,8 @@
     <sheet name="11_Roles" sheetId="13" r:id="rId11"/>
     <sheet name="12_Language Labels" sheetId="15" r:id="rId12"/>
     <sheet name="13_Authority Sources" sheetId="16" r:id="rId13"/>
+    <sheet name="14_Traditional Knowledge Labels" sheetId="17" r:id="rId14"/>
+    <sheet name="15_Biocultural Labels" sheetId="18" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="865">
   <si>
     <t>Term ID</t>
   </si>
@@ -2294,12 +2296,377 @@
 with works that are already free of known copyright
 restrictions throughout the world.</t>
   </si>
+  <si>
+    <t>TK Attribution (TK A)</t>
+  </si>
+  <si>
+    <t>This Label is being used to correct historical mistakes or exclusions pertaining to this material. This is especially in relation to the names of the people involved in performing or making this work and/or correctly naming the community from which it originally derives. As a user you are being asked to also apply the correct attribution in any future use of this work.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-attribution/</t>
+  </si>
+  <si>
+    <t>TK Clan (TK CL)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available. The Label lets future users know that this material has specific conditions for use and sharing because of clan membership and/or relationships. This material is not, and never was, free, public, or available for everyone. This Label asks viewers of these materials to respect the cultural values and expectations about circulation and use defined by designated clans, members, and their internal relations.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-clan/</t>
+  </si>
+  <si>
+    <t>TK Family (TK F)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available. The Label is correcting a misunderstanding about the circulation options for this material and letting any users know that this material has specific conditions for sharing between family members. Who these family members are, and how sharing occurs will be defined in each locale. This material is not, and never was, free, public, or available for everyone at anytime. This Label asks you to think about how you are going to use this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>TK Multiple Communities (TK MC)</t>
+  </si>
+  <si>
+    <t>Responsibility and ownership over this material is spread across several distinct communities. Use will be dependent upon discussion and negotiation with the multiple communities named herein [insert names]. Decisions about use will need to be decided collectively. As an external user of this material you are asked to recognize and respect cultural protocols in relation to the use of this material and clear your intended use with the relevant communities.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-multiple-communities/</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-family/</t>
+  </si>
+  <si>
+    <t>TK Community Voice (TK CV)</t>
+  </si>
+  <si>
+    <t>This Label is being used to encourage the sharing of stories and voices about this material. The Label indicates that existing knowledge or descriptions are incomplete or partial. Any community member is invited and welcome to contribute to our community knowledge about this event, photograph, recording or heritage item. Sharing our voices helps us reclaim our histories and knowledge. This sharing is an internal process.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-community-voice/</t>
+  </si>
+  <si>
+    <t>TK Creative (TK CR)</t>
+  </si>
+  <si>
+    <t>This Label is being used to acknowledge the relationship between the creative practices of [name] and [community name] and the associated cultural responsibilities.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-creative/</t>
+  </si>
+  <si>
+    <t>TK Verified (TK V)</t>
+  </si>
+  <si>
+    <t>This Label affirms that the representation and presentation of this material is in keeping with community expectations and cultural protocols. It lets you know that for the individual, family or community represented in this material, use is considered fair, reasonable and respectful.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-verified/</t>
+  </si>
+  <si>
+    <t>TK Non-Verified (TK NV)</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-non-verified/</t>
+  </si>
+  <si>
+    <t>This Label is being used because there are concerns about accuracy and/or representations made in this material. This material was not created through informed consent or community protocols for research and engagement. Therefore, questions about its accuracy and who/how it represents this community are being raised.</t>
+  </si>
+  <si>
+    <t>TK Seasonal (TK S)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material traditionally and usually is heard and/or utilized at a particular time of year and in response to specific seasonal changes and conditions. For instance, many important ceremonies are held at very specific times of the year. This Label is being used to indicate sophisticated relationships between land and knowledge creation. It is also being used to highlight the relationships between recorded material and the specific contexts where it derives, especially the interconnected and embodied teachings that it conveys.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-seasonal/</t>
+  </si>
+  <si>
+    <t>This material has specific gender restrictions on access. It is usually only to be accessed and used by women in the community. If you are not from the community and you have accessed this material, you are requested not to download, copy, remix or otherwise circulate this material to others without permission. This Label asks you to think about whether you should be using this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>TK Women General (TK WG)</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-women-general/</t>
+  </si>
+  <si>
+    <t>TK Men General (TK MG)</t>
+  </si>
+  <si>
+    <t>This material has specific gender restrictions on access. It is usually only to be accessed and used by men in the community. If you are not from the community and you have accessed this material, you are requested to not download, copy, remix or otherwise circulate this material to others without permission. This Label asks you to think about whether you should be using this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-men-general/</t>
+  </si>
+  <si>
+    <t>TK Men Restricted (TK MR)</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-men-restricted/</t>
+  </si>
+  <si>
+    <t>This material has specific gender restrictions on access. It is regarded as important secret and/or ceremonial material that has community-based laws in relation to who can access it. Given its nature it is only to be accessed and used by authorized [and/or initiated] men in the community. If you are an external third party user and you have accessed this material, you are requested to not download, copy, remix or otherwise circulate this material to others. This material is not freely available within the community and it therefore should not be considered freely available outside of the community. This Label asks you to think about whether you should be using this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-women-restricted/</t>
+  </si>
+  <si>
+    <t>TK Women Restricted (TK WR)</t>
+  </si>
+  <si>
+    <t>This material has specific gender restrictions on access. It is regarded as important secret and/or ceremonial material that has community-based laws in relation to who can access it. Given its nature it is only to be accessed and used by authorized [and/or initiated] women in the community. If you are an external third party user and you have accessed this material, you are requested to not download, copy, remix or otherwise circulate this material to others. This material is not freely available within the community and it therefore should not be considered freely available outside of the community. This Label asks you to think about whether you should be using this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>TK Culturally Sensitive (TK CS)</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-culturally-sensitive/</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material has cultural and/or historical sensitivities. The Label asks for care to be taken when this material is accessed, used, and circulated, especially when materials are first returned or reunited with communities of origin. In some instances, this Label will indicate that there are specific permissions for use of this material required directly from the community itself.</t>
+  </si>
+  <si>
+    <t>TK Secret / Sacred (TK SS)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available because it contains important secret or sacred components. The Label is correcting a misunderstanding about the significance of this material and therefore its circulation conditions. It is letting users know that because of its secret/sacred status it is not, and was never free, public, or available for everyone at anytime. This Label asks you to think about whether you should be using this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-secret-sacred/</t>
+  </si>
+  <si>
+    <t>TK Open to Commercialization (TK OC)</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-commercial/</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that [community name or authorized party] is open to commercialization opportunities that might derive from any cultural material with traditional knowledge to which this Label is connected to. As a primary party for any partnership and collaboration opportunities that emerge from the use of this cultural material and traditional knowledge, we retain an expressed interest in any future negotiations.</t>
+  </si>
+  <si>
+    <t>TK Non-Commercial (TK NC)</t>
+  </si>
+  <si>
+    <t>This material has been designated as being available for non-commercial use. You are allowed to use this material for non-commercial purposes including for research, study, or public presentation and/or online in blogs or non-commercial websites. This Label asks you to think and act with fairness and responsibility towards this material and the original custodians.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-non-commercial/</t>
+  </si>
+  <si>
+    <t>TK Community Use Only (TK CO)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available. The Label is correcting a misunderstanding about the circulation options for this material and letting any users know that this material has specific conditions for circulation within the community. It is not, and never was, free, public, or available for everyone at anytime. This Label asks you to think about how you are going to use this material and to respect different cultural values and expectations about circulation and use.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-community-use-only/</t>
+  </si>
+  <si>
+    <t>TK Outreach (TK O)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available. The Label is correcting a misunderstanding about the circulation options for this material and letting any users know that this material can be used for educational outreach activities. This Label asks you to respect the designated circulation conditions for this material and additionally, where possible, to develop a means for fair and equitable reciprocal exchange for the use of this material with the relevant TK holders. This exchange might include access to educational or other resources that are difficult to access under normal circumstances.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-outreach/</t>
+  </si>
+  <si>
+    <t>TK Open to Collaboration (TK CB)</t>
+  </si>
+  <si>
+    <t>This Label is being used to make clear [community name or authorizing body] is open to future engagement, collaboration, and partnership around research opportunities.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/tk-open-to-collaboration/</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>tka</t>
+  </si>
+  <si>
+    <t>tkcl</t>
+  </si>
+  <si>
+    <t>tkf</t>
+  </si>
+  <si>
+    <t>tkmc</t>
+  </si>
+  <si>
+    <t>tkcv</t>
+  </si>
+  <si>
+    <t>tkcr</t>
+  </si>
+  <si>
+    <t>tkv</t>
+  </si>
+  <si>
+    <t>tknv</t>
+  </si>
+  <si>
+    <t>tks</t>
+  </si>
+  <si>
+    <t>tkwg</t>
+  </si>
+  <si>
+    <t>tkmg</t>
+  </si>
+  <si>
+    <t>tkmr</t>
+  </si>
+  <si>
+    <t>tkwr</t>
+  </si>
+  <si>
+    <t>tkcs</t>
+  </si>
+  <si>
+    <t>tkss</t>
+  </si>
+  <si>
+    <t>tkoc</t>
+  </si>
+  <si>
+    <t>tknc</t>
+  </si>
+  <si>
+    <t>tkco</t>
+  </si>
+  <si>
+    <t>tko</t>
+  </si>
+  <si>
+    <t>tkcb</t>
+  </si>
+  <si>
+    <t>BC Provenance (BC P)</t>
+  </si>
+  <si>
+    <t>This Label is being used to affirm an inherent interest Indigenous people have in the scientific collections and data about communities, peoples, and the biodiversity found within traditional lands, waters and territories. [Community name or authorizing party] retains the right to be named and associated with it into the future. This association reflects a significant relationship and responsibility to [the species or biological entity] and associated scientific collections and data.
+[Optional attribution statement]</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-provenance/</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-multiple-communities/</t>
+  </si>
+  <si>
+    <t>BC Multiple Communities (BC MC)</t>
+  </si>
+  <si>
+    <t>This Label is being used to affirm that responsibility and ownership over this information, collection, data, and digital sequence information (DSI) is spread across several distinct communities. Use will be dependent upon discussion and negotiation with these multiple communities.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-clan/</t>
+  </si>
+  <si>
+    <t>BC Clan (BC CL)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that this material is traditionally and usually not publicly available. The Label lets future users know that this data has specific conditions for use and sharing because of clan membership and/or relationships. This Label asks viewers of this data to respect the cultural values and expectations about circulation and use defined by designated clans, members, and their internal relations.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-consent-verified/</t>
+  </si>
+  <si>
+    <t>BC Consent Verified (BC CV)</t>
+  </si>
+  <si>
+    <t>This Label is being used to verify that [community name or authorizing party] have consent conditions in place for the use of this information, collections, data, and digital sequence information. [These can be found at ….].</t>
+  </si>
+  <si>
+    <t>BC Consent Non-Verified (BC CNV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This Label is being used because there are concerns about the accuracy of the consent and/or representations made for this data. This material was not created through informed consent or community protocols for research and engagement. </t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-consent-non-verified/</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-research-use/</t>
+  </si>
+  <si>
+    <t>This Label is being used by [community name or authorizing body] to allow this information, collection, data, and digital sequence information (DSI) to be used for unspecified research purposes. This Label does not provide permission for commercialization activities.
+[Optional return of research results statement]</t>
+  </si>
+  <si>
+    <t>BC Research Use (BC R)</t>
+  </si>
+  <si>
+    <t>This Label is being used to make clear [community name or authorizing body] is open to future engagement, collaboration, and partnership around research and outreach opportunities.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-open-to-collaboration/</t>
+  </si>
+  <si>
+    <t>BC Open to Collaboration (BC CB)</t>
+  </si>
+  <si>
+    <t>BC Open to Commercialization (BC OC)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that [community name or authorizing party] is open to commercialization opportunities that might derive from any information, collections, data, and digital sequence information (DSI) to which this Label is connected. As a primary party in any partnership and collaboration opportunity that emerges from the use of these resources, we retain an express interest in any future negotiations.</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-open-to-commercialization/</t>
+  </si>
+  <si>
+    <t>BC Outreach (BC O)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Label is letting any users know that this data can be used for educational outreach activities. This Label asks you to respect the designated circulation conditions for these biocultural materials and/or data and additionally, where possible, to develop a means for fair and equitable reciprocal exchange for the use of this data with the relevant BC holders. </t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-outreach/</t>
+  </si>
+  <si>
+    <t>https://localcontexts.org/label/bc-non-commercial/</t>
+  </si>
+  <si>
+    <t>BC Non-Commercial (BC NC)</t>
+  </si>
+  <si>
+    <t>This Label is being used to indicate that these biocultural materials and/or data have been designated as being available for non-commercial use. You are allowed to use this material for non-commercial purposes including for research, study, or public presentation and/or online in blogs or non-commercial websites. This Label asks you to think and act with respect and responsibility towards this data and the original custodians.</t>
+  </si>
+  <si>
+    <t>bcp</t>
+  </si>
+  <si>
+    <t>bcmc</t>
+  </si>
+  <si>
+    <t>bccl</t>
+  </si>
+  <si>
+    <t>bccv</t>
+  </si>
+  <si>
+    <t>bccnv</t>
+  </si>
+  <si>
+    <t>bcr</t>
+  </si>
+  <si>
+    <t>bccb</t>
+  </si>
+  <si>
+    <t>bcoc</t>
+  </si>
+  <si>
+    <t>bco</t>
+  </si>
+  <si>
+    <t>bcnc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2364,6 +2731,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF44474A"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2397,7 +2770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2412,6 +2785,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{7D5AF2CA-6FAC-4DED-9EC5-A1BA931E1331}"/>
@@ -4858,6 +5237,550 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F67E00-EC1B-4E47-80B8-6C2ADC61550B}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>805</v>
+      </c>
+      <c r="B3" t="s">
+        <v>744</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>745</v>
+      </c>
+      <c r="F3" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>806</v>
+      </c>
+      <c r="B4" t="s">
+        <v>747</v>
+      </c>
+      <c r="C4" t="s">
+        <v>748</v>
+      </c>
+      <c r="F4" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B5" t="s">
+        <v>750</v>
+      </c>
+      <c r="C5" t="s">
+        <v>751</v>
+      </c>
+      <c r="F5" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>808</v>
+      </c>
+      <c r="B6" t="s">
+        <v>752</v>
+      </c>
+      <c r="C6" t="s">
+        <v>753</v>
+      </c>
+      <c r="F6" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>809</v>
+      </c>
+      <c r="B7" t="s">
+        <v>756</v>
+      </c>
+      <c r="C7" t="s">
+        <v>757</v>
+      </c>
+      <c r="F7" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>810</v>
+      </c>
+      <c r="B8" t="s">
+        <v>759</v>
+      </c>
+      <c r="C8" t="s">
+        <v>760</v>
+      </c>
+      <c r="F8" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>811</v>
+      </c>
+      <c r="B9" t="s">
+        <v>762</v>
+      </c>
+      <c r="C9" t="s">
+        <v>763</v>
+      </c>
+      <c r="F9" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>812</v>
+      </c>
+      <c r="B10" t="s">
+        <v>765</v>
+      </c>
+      <c r="C10" t="s">
+        <v>767</v>
+      </c>
+      <c r="F10" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>813</v>
+      </c>
+      <c r="B11" t="s">
+        <v>768</v>
+      </c>
+      <c r="C11" t="s">
+        <v>769</v>
+      </c>
+      <c r="F11" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>814</v>
+      </c>
+      <c r="B12" t="s">
+        <v>772</v>
+      </c>
+      <c r="C12" t="s">
+        <v>771</v>
+      </c>
+      <c r="F12" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>815</v>
+      </c>
+      <c r="B13" t="s">
+        <v>774</v>
+      </c>
+      <c r="C13" t="s">
+        <v>775</v>
+      </c>
+      <c r="F13" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>816</v>
+      </c>
+      <c r="B14" t="s">
+        <v>777</v>
+      </c>
+      <c r="C14" t="s">
+        <v>779</v>
+      </c>
+      <c r="F14" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>817</v>
+      </c>
+      <c r="B15" t="s">
+        <v>781</v>
+      </c>
+      <c r="C15" t="s">
+        <v>782</v>
+      </c>
+      <c r="F15" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>818</v>
+      </c>
+      <c r="B16" t="s">
+        <v>783</v>
+      </c>
+      <c r="C16" t="s">
+        <v>785</v>
+      </c>
+      <c r="F16" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>819</v>
+      </c>
+      <c r="B17" t="s">
+        <v>786</v>
+      </c>
+      <c r="C17" t="s">
+        <v>787</v>
+      </c>
+      <c r="F17" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>820</v>
+      </c>
+      <c r="B18" t="s">
+        <v>789</v>
+      </c>
+      <c r="C18" t="s">
+        <v>791</v>
+      </c>
+      <c r="F18" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>821</v>
+      </c>
+      <c r="B19" t="s">
+        <v>792</v>
+      </c>
+      <c r="C19" t="s">
+        <v>793</v>
+      </c>
+      <c r="F19" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>822</v>
+      </c>
+      <c r="B20" t="s">
+        <v>795</v>
+      </c>
+      <c r="C20" t="s">
+        <v>796</v>
+      </c>
+      <c r="F20" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>823</v>
+      </c>
+      <c r="B21" t="s">
+        <v>798</v>
+      </c>
+      <c r="C21" t="s">
+        <v>799</v>
+      </c>
+      <c r="F21" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>824</v>
+      </c>
+      <c r="B22" t="s">
+        <v>801</v>
+      </c>
+      <c r="C22" t="s">
+        <v>802</v>
+      </c>
+      <c r="F22" t="s">
+        <v>803</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3B1DC4-7228-4E7B-AE10-2426AE58FF55}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13">
+        <v>5</v>
+      </c>
+      <c r="F1" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>855</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>825</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>826</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>856</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>829</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>830</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>857</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>832</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>833</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>858</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>835</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>836</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>859</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>837</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>860</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>842</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>841</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>861</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>845</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>843</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>862</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>846</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>847</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>863</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>849</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>850</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>853</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>854</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>852</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{1F779799-C8B2-499C-B7ED-E33915A311AB}"/>
+    <hyperlink ref="F12" r:id="rId2" xr:uid="{C28B5BEF-4771-4915-BA25-24C55EFF2E13}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477AB8E0-193B-4ACE-9281-1EB5DE711D3C}">
   <dimension ref="A1:F32"/>
@@ -5245,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16B73E5-B011-40A2-8AFF-3FBA72B05675}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
saved changes before merge
</commit_message>
<xml_diff>
--- a/xlsx/Lists.xlsx
+++ b/xlsx/Lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A227B620-8B34-4065-B621-0B50314FD73C}"/>
+  <xr:revisionPtr revIDLastSave="405" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88ED991A-AE5C-4BF0-A97E-FF7025AB0314}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_Languages" sheetId="2" r:id="rId1"/>
@@ -1999,9 +1999,6 @@
     <t>reg_02</t>
   </si>
   <si>
-    <t>Asia Pasific</t>
-  </si>
-  <si>
     <t>reg_03</t>
   </si>
   <si>
@@ -2666,6 +2663,9 @@
   </si>
   <si>
     <t>GA_lang</t>
+  </si>
+  <si>
+    <t>Asia Pacific</t>
   </si>
 </sst>
 </file>
@@ -3080,7 +3080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7DCC5-93A4-4F15-9716-2215F2C5540F}">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
@@ -3614,10 +3614,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -4930,8 +4930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539D0DAF-3B47-4A29-A75D-3D6ADB320449}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4989,39 +4989,39 @@
         <v>648</v>
       </c>
       <c r="B4" t="s">
-        <v>649</v>
+        <v>866</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>651</v>
+      </c>
+      <c r="B7" t="s">
         <v>652</v>
-      </c>
-      <c r="B7" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>653</v>
+      </c>
+      <c r="B8" t="s">
         <v>654</v>
-      </c>
-      <c r="B8" t="s">
-        <v>655</v>
       </c>
     </row>
   </sheetData>
@@ -5061,58 +5061,58 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B2" t="s">
         <v>680</v>
-      </c>
-      <c r="B2" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B3" t="s">
         <v>682</v>
-      </c>
-      <c r="B3" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>683</v>
+      </c>
+      <c r="B4" t="s">
         <v>684</v>
-      </c>
-      <c r="B4" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>685</v>
+      </c>
+      <c r="B5" t="s">
         <v>686</v>
-      </c>
-      <c r="B5" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>687</v>
+      </c>
+      <c r="B6" t="s">
         <v>688</v>
-      </c>
-      <c r="B6" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>689</v>
+      </c>
+      <c r="B7" t="s">
         <v>690</v>
-      </c>
-      <c r="B7" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>691</v>
+      </c>
+      <c r="B8" t="s">
         <v>692</v>
-      </c>
-      <c r="B8" t="s">
-        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -5152,18 +5152,18 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -5204,46 +5204,46 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
   </sheetData>
@@ -5304,287 +5304,287 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>744</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="F3" t="s">
         <v>745</v>
-      </c>
-      <c r="F3" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B4" t="s">
+        <v>746</v>
+      </c>
+      <c r="C4" t="s">
         <v>747</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>748</v>
-      </c>
-      <c r="F4" t="s">
-        <v>749</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B5" t="s">
+        <v>749</v>
+      </c>
+      <c r="C5" t="s">
         <v>750</v>
       </c>
-      <c r="C5" t="s">
-        <v>751</v>
-      </c>
       <c r="F5" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B6" t="s">
+        <v>751</v>
+      </c>
+      <c r="C6" t="s">
         <v>752</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>753</v>
-      </c>
-      <c r="F6" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="B7" t="s">
+        <v>755</v>
+      </c>
+      <c r="C7" t="s">
         <v>756</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>757</v>
-      </c>
-      <c r="F7" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="B8" t="s">
+        <v>758</v>
+      </c>
+      <c r="C8" t="s">
         <v>759</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>760</v>
-      </c>
-      <c r="F8" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="B9" t="s">
+        <v>761</v>
+      </c>
+      <c r="C9" t="s">
         <v>762</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>763</v>
-      </c>
-      <c r="F9" t="s">
-        <v>764</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="B10" t="s">
+        <v>764</v>
+      </c>
+      <c r="C10" t="s">
+        <v>766</v>
+      </c>
+      <c r="F10" t="s">
         <v>765</v>
-      </c>
-      <c r="C10" t="s">
-        <v>767</v>
-      </c>
-      <c r="F10" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B11" t="s">
+        <v>767</v>
+      </c>
+      <c r="C11" t="s">
         <v>768</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>769</v>
-      </c>
-      <c r="F11" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B12" t="s">
+        <v>771</v>
+      </c>
+      <c r="C12" t="s">
+        <v>770</v>
+      </c>
+      <c r="F12" t="s">
         <v>772</v>
-      </c>
-      <c r="C12" t="s">
-        <v>771</v>
-      </c>
-      <c r="F12" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B13" t="s">
+        <v>773</v>
+      </c>
+      <c r="C13" t="s">
         <v>774</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>775</v>
-      </c>
-      <c r="F13" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B14" t="s">
+        <v>776</v>
+      </c>
+      <c r="C14" t="s">
+        <v>778</v>
+      </c>
+      <c r="F14" t="s">
         <v>777</v>
-      </c>
-      <c r="C14" t="s">
-        <v>779</v>
-      </c>
-      <c r="F14" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B15" t="s">
+        <v>780</v>
+      </c>
+      <c r="C15" t="s">
         <v>781</v>
       </c>
-      <c r="C15" t="s">
-        <v>782</v>
-      </c>
       <c r="F15" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B16" t="s">
+        <v>782</v>
+      </c>
+      <c r="C16" t="s">
+        <v>784</v>
+      </c>
+      <c r="F16" t="s">
         <v>783</v>
-      </c>
-      <c r="C16" t="s">
-        <v>785</v>
-      </c>
-      <c r="F16" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B17" t="s">
+        <v>785</v>
+      </c>
+      <c r="C17" t="s">
         <v>786</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
         <v>787</v>
-      </c>
-      <c r="F17" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="B18" t="s">
+        <v>788</v>
+      </c>
+      <c r="C18" t="s">
+        <v>790</v>
+      </c>
+      <c r="F18" t="s">
         <v>789</v>
-      </c>
-      <c r="C18" t="s">
-        <v>791</v>
-      </c>
-      <c r="F18" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="B19" t="s">
+        <v>791</v>
+      </c>
+      <c r="C19" t="s">
         <v>792</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
         <v>793</v>
-      </c>
-      <c r="F19" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B20" t="s">
+        <v>794</v>
+      </c>
+      <c r="C20" t="s">
         <v>795</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
         <v>796</v>
-      </c>
-      <c r="F20" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="B21" t="s">
+        <v>797</v>
+      </c>
+      <c r="C21" t="s">
         <v>798</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
         <v>799</v>
-      </c>
-      <c r="F21" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B22" t="s">
+        <v>800</v>
+      </c>
+      <c r="C22" t="s">
         <v>801</v>
       </c>
-      <c r="C22" t="s">
+      <c r="F22" t="s">
         <v>802</v>
-      </c>
-      <c r="F22" t="s">
-        <v>803</v>
       </c>
     </row>
   </sheetData>
@@ -5643,147 +5643,147 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B3" t="s">
+        <v>824</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>825</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>826</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B4" t="s">
+        <v>828</v>
+      </c>
+      <c r="C4" t="s">
         <v>829</v>
       </c>
-      <c r="C4" t="s">
-        <v>830</v>
-      </c>
       <c r="F4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B5" t="s">
+        <v>831</v>
+      </c>
+      <c r="C5" t="s">
         <v>832</v>
       </c>
-      <c r="C5" t="s">
-        <v>833</v>
-      </c>
       <c r="F5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B6" t="s">
+        <v>834</v>
+      </c>
+      <c r="C6" t="s">
         <v>835</v>
       </c>
-      <c r="C6" t="s">
-        <v>836</v>
-      </c>
       <c r="F6" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B7" t="s">
+        <v>836</v>
+      </c>
+      <c r="C7" t="s">
         <v>837</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>838</v>
-      </c>
-      <c r="F7" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B8" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C8" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F8" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C9" t="s">
+        <v>842</v>
+      </c>
+      <c r="F9" t="s">
         <v>843</v>
-      </c>
-      <c r="F9" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B10" t="s">
+        <v>845</v>
+      </c>
+      <c r="C10" t="s">
         <v>846</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>847</v>
-      </c>
-      <c r="F10" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B11" t="s">
+        <v>848</v>
+      </c>
+      <c r="C11" t="s">
         <v>849</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>850</v>
-      </c>
-      <c r="F11" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B12" t="s">
+        <v>852</v>
+      </c>
+      <c r="C12" t="s">
         <v>853</v>
       </c>
-      <c r="C12" t="s">
-        <v>854</v>
-      </c>
       <c r="F12" s="11" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
   </sheetData>
@@ -5800,7 +5800,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6909,10 +6909,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C3" t="s">
         <v>479</v>
@@ -6920,21 +6920,21 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B5" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C5" t="s">
         <v>483</v>
@@ -6942,10 +6942,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C6" t="s">
         <v>482</v>
@@ -6953,10 +6953,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B7" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C7" t="s">
         <v>481</v>
@@ -6964,10 +6964,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B8" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C8" t="s">
         <v>480</v>
@@ -6975,134 +6975,134 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B9" t="s">
+        <v>655</v>
+      </c>
+      <c r="C9" t="s">
         <v>656</v>
-      </c>
-      <c r="C9" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B10" t="s">
+        <v>661</v>
+      </c>
+      <c r="C10" t="s">
         <v>662</v>
-      </c>
-      <c r="C10" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B11" t="s">
+        <v>657</v>
+      </c>
+      <c r="C11" t="s">
         <v>658</v>
-      </c>
-      <c r="C11" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B12" t="s">
+        <v>663</v>
+      </c>
+      <c r="C12" t="s">
         <v>664</v>
-      </c>
-      <c r="C12" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B13" t="s">
+        <v>659</v>
+      </c>
+      <c r="C13" t="s">
         <v>660</v>
-      </c>
-      <c r="C13" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B14" t="s">
+        <v>667</v>
+      </c>
+      <c r="C14" t="s">
         <v>668</v>
-      </c>
-      <c r="C14" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B15" t="s">
+        <v>665</v>
+      </c>
+      <c r="C15" t="s">
         <v>666</v>
-      </c>
-      <c r="C15" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B16" t="s">
+        <v>669</v>
+      </c>
+      <c r="C16" t="s">
         <v>670</v>
-      </c>
-      <c r="C16" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B17" t="s">
+        <v>671</v>
+      </c>
+      <c r="C17" t="s">
         <v>672</v>
-      </c>
-      <c r="C17" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B18" t="s">
+        <v>675</v>
+      </c>
+      <c r="C18" t="s">
         <v>676</v>
-      </c>
-      <c r="C18" t="s">
-        <v>677</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B19" t="s">
+        <v>677</v>
+      </c>
+      <c r="C19" t="s">
         <v>678</v>
-      </c>
-      <c r="C19" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B20" t="s">
+        <v>673</v>
+      </c>
+      <c r="C20" t="s">
         <v>674</v>
-      </c>
-      <c r="C20" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7110,21 +7110,21 @@
         <v>484</v>
       </c>
       <c r="B21" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C21" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B22" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C22" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -8014,10 +8014,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>711</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>712</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated prj list. exresource element, list, ui added
</commit_message>
<xml_diff>
--- a/xlsx/Lists.xlsx
+++ b/xlsx/Lists.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88ED991A-AE5C-4BF0-A97E-FF7025AB0314}"/>
+  <xr:revisionPtr revIDLastSave="489" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDB1C0EE-FF7D-4E2A-BA14-DDF394921354}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="984" yWindow="1008" windowWidth="8076" windowHeight="10044" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="01_Languages" sheetId="2" r:id="rId1"/>
-    <sheet name="02_Themes" sheetId="3" r:id="rId2"/>
-    <sheet name="03_Cultural Context" sheetId="4" r:id="rId3"/>
-    <sheet name="04_Social Groups" sheetId="5" r:id="rId4"/>
-    <sheet name="05_Rights" sheetId="6" r:id="rId5"/>
-    <sheet name="06_Gender" sheetId="7" r:id="rId6"/>
-    <sheet name="07_Cultural Sensitivity" sheetId="8" r:id="rId7"/>
-    <sheet name="08_Occupations" sheetId="9" r:id="rId8"/>
-    <sheet name="09_Project Types" sheetId="10" r:id="rId9"/>
-    <sheet name="10_Project Regions" sheetId="11" r:id="rId10"/>
-    <sheet name="11_Roles" sheetId="13" r:id="rId11"/>
-    <sheet name="12_Language Labels" sheetId="15" r:id="rId12"/>
-    <sheet name="13_Authority Sources" sheetId="16" r:id="rId13"/>
-    <sheet name="14_Traditional Knowledge Labels" sheetId="17" r:id="rId14"/>
-    <sheet name="15_Biocultural Labels" sheetId="18" r:id="rId15"/>
+    <sheet name="01_Languages (OBJ,ENT)" sheetId="2" r:id="rId1"/>
+    <sheet name="02_Themes (OBJ)" sheetId="3" r:id="rId2"/>
+    <sheet name="03_Cultural Context (OBJ)" sheetId="4" r:id="rId3"/>
+    <sheet name="04_Social Groups (OBJ)" sheetId="5" r:id="rId4"/>
+    <sheet name="05_Rights (OBJ)" sheetId="6" r:id="rId5"/>
+    <sheet name="06_Gender (ENT)" sheetId="7" r:id="rId6"/>
+    <sheet name="07_Cultural Sensitivity (OBJ)" sheetId="8" r:id="rId7"/>
+    <sheet name="08_Occupations (ENT)" sheetId="9" r:id="rId8"/>
+    <sheet name="09_Project Types (COL)" sheetId="10" r:id="rId9"/>
+    <sheet name="10_Project Regions (COL)" sheetId="11" r:id="rId10"/>
+    <sheet name="11_Roles (ENT)" sheetId="13" r:id="rId11"/>
+    <sheet name="12_Language Labels (OBJ,ENT)" sheetId="15" r:id="rId12"/>
+    <sheet name="13_Authority Sources (ENT)" sheetId="16" r:id="rId13"/>
+    <sheet name="14_TraditionalKnowledge (OBJ)" sheetId="17" r:id="rId14"/>
+    <sheet name="15_Biocultural Labels (OBJ)" sheetId="18" r:id="rId15"/>
+    <sheet name="16_External Resources" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="875">
   <si>
     <t>Term ID</t>
   </si>
@@ -2666,6 +2667,30 @@
   </si>
   <si>
     <t>Asia Pacific</t>
+  </si>
+  <si>
+    <t>exres_01</t>
+  </si>
+  <si>
+    <t>exres_02</t>
+  </si>
+  <si>
+    <t>exres_03</t>
+  </si>
+  <si>
+    <t>exres_04</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Exhibition</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Interactive Form</t>
   </si>
 </sst>
 </file>
@@ -2809,10 +2834,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3078,18 +3099,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7DCC5-93A4-4F15-9716-2215F2C5540F}">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -3110,7 +3135,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3131,7 +3156,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3144,7 +3169,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3157,7 +3182,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3170,7 +3195,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,7 +3208,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3196,7 +3221,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -3209,7 +3234,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3222,7 +3247,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3235,7 +3260,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -3248,7 +3273,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -3261,7 +3286,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -3272,9 +3297,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -3285,9 +3309,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -3298,9 +3322,8 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3310,10 +3333,8 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -3324,9 +3345,8 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
@@ -3337,9 +3357,8 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -3350,9 +3369,8 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -3363,9 +3381,8 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
@@ -3376,9 +3393,8 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>47</v>
       </c>
@@ -3389,9 +3405,8 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>49</v>
       </c>
@@ -3404,7 +3419,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
@@ -3417,7 +3432,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>53</v>
       </c>
@@ -3430,7 +3445,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
@@ -3443,7 +3458,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
@@ -3456,7 +3471,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>59</v>
       </c>
@@ -3469,7 +3484,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>61</v>
       </c>
@@ -3482,7 +3497,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -3495,7 +3510,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -3508,7 +3523,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>67</v>
       </c>
@@ -3521,7 +3536,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>69</v>
       </c>
@@ -3534,7 +3549,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -3547,7 +3562,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -3560,7 +3575,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>75</v>
       </c>
@@ -3573,7 +3588,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -3586,7 +3601,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>78</v>
       </c>
@@ -3599,7 +3614,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>80</v>
       </c>
@@ -3612,7 +3627,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>865</v>
       </c>
@@ -3625,7 +3640,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>82</v>
       </c>
@@ -3638,7 +3653,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>84</v>
       </c>
@@ -3651,7 +3666,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
@@ -3664,7 +3679,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>88</v>
       </c>
@@ -3677,7 +3692,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>90</v>
       </c>
@@ -3690,7 +3705,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>92</v>
       </c>
@@ -3703,7 +3718,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
@@ -3716,7 +3731,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>96</v>
       </c>
@@ -3729,7 +3744,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>98</v>
       </c>
@@ -3742,7 +3757,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
@@ -3755,7 +3770,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>102</v>
       </c>
@@ -3768,7 +3783,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>104</v>
       </c>
@@ -3781,7 +3796,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>106</v>
       </c>
@@ -3794,7 +3809,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>108</v>
       </c>
@@ -3807,7 +3822,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>110</v>
       </c>
@@ -3820,7 +3835,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>112</v>
       </c>
@@ -3833,7 +3848,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>114</v>
       </c>
@@ -3846,7 +3861,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>116</v>
       </c>
@@ -3859,7 +3874,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>118</v>
       </c>
@@ -3872,7 +3887,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>120</v>
       </c>
@@ -3885,7 +3900,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>122</v>
       </c>
@@ -3898,7 +3913,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>124</v>
       </c>
@@ -3911,7 +3926,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>126</v>
       </c>
@@ -3924,7 +3939,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>128</v>
       </c>
@@ -3937,7 +3952,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>130</v>
       </c>
@@ -3950,7 +3965,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>132</v>
       </c>
@@ -3963,7 +3978,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>134</v>
       </c>
@@ -3976,7 +3991,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>136</v>
       </c>
@@ -3989,7 +4004,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -4002,7 +4017,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>140</v>
       </c>
@@ -4015,7 +4030,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>142</v>
       </c>
@@ -4028,7 +4043,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>144</v>
       </c>
@@ -4041,7 +4056,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>146</v>
       </c>
@@ -4054,7 +4069,7 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>148</v>
       </c>
@@ -4067,7 +4082,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>150</v>
       </c>
@@ -4080,7 +4095,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>152</v>
       </c>
@@ -4093,7 +4108,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>154</v>
       </c>
@@ -4106,7 +4121,7 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>156</v>
       </c>
@@ -4119,7 +4134,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>158</v>
       </c>
@@ -4132,7 +4147,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>160</v>
       </c>
@@ -4145,7 +4160,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>162</v>
       </c>
@@ -4158,7 +4173,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>164</v>
       </c>
@@ -4171,7 +4186,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>166</v>
       </c>
@@ -4184,7 +4199,7 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>167</v>
       </c>
@@ -4197,7 +4212,7 @@
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>169</v>
       </c>
@@ -4210,7 +4225,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>171</v>
       </c>
@@ -4223,7 +4238,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>173</v>
       </c>
@@ -4236,7 +4251,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>175</v>
       </c>
@@ -4249,7 +4264,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>177</v>
       </c>
@@ -4262,7 +4277,7 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>179</v>
       </c>
@@ -4275,7 +4290,7 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>181</v>
       </c>
@@ -4288,7 +4303,7 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>183</v>
       </c>
@@ -4301,7 +4316,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>185</v>
       </c>
@@ -4314,7 +4329,7 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>187</v>
       </c>
@@ -4327,7 +4342,7 @@
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>189</v>
       </c>
@@ -4340,7 +4355,7 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>191</v>
       </c>
@@ -4353,7 +4368,7 @@
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>193</v>
       </c>
@@ -4366,7 +4381,7 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>195</v>
       </c>
@@ -4379,7 +4394,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>197</v>
       </c>
@@ -4392,7 +4407,7 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>199</v>
       </c>
@@ -4405,7 +4420,7 @@
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>201</v>
       </c>
@@ -4418,7 +4433,7 @@
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>203</v>
       </c>
@@ -4431,7 +4446,7 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>205</v>
       </c>
@@ -4444,7 +4459,7 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>207</v>
       </c>
@@ -4457,7 +4472,7 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>209</v>
       </c>
@@ -4470,7 +4485,7 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>211</v>
       </c>
@@ -4483,7 +4498,7 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>213</v>
       </c>
@@ -4496,7 +4511,7 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>215</v>
       </c>
@@ -4509,7 +4524,7 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>217</v>
       </c>
@@ -4522,7 +4537,7 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>219</v>
       </c>
@@ -4535,7 +4550,7 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>221</v>
       </c>
@@ -4548,7 +4563,7 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>223</v>
       </c>
@@ -4561,7 +4576,7 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>225</v>
       </c>
@@ -4574,7 +4589,7 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>227</v>
       </c>
@@ -4587,7 +4602,7 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>229</v>
       </c>
@@ -4600,7 +4615,7 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>231</v>
       </c>
@@ -4613,7 +4628,7 @@
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>233</v>
       </c>
@@ -4626,7 +4641,7 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>235</v>
       </c>
@@ -4639,7 +4654,7 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>237</v>
       </c>
@@ -4652,7 +4667,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>239</v>
       </c>
@@ -4665,7 +4680,7 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>241</v>
       </c>
@@ -4678,7 +4693,7 @@
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>243</v>
       </c>
@@ -4691,7 +4706,7 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>245</v>
       </c>
@@ -4704,7 +4719,7 @@
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>247</v>
       </c>
@@ -4717,7 +4732,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>248</v>
       </c>
@@ -4730,7 +4745,7 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>250</v>
       </c>
@@ -4743,7 +4758,7 @@
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>252</v>
       </c>
@@ -4756,7 +4771,7 @@
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>254</v>
       </c>
@@ -4769,7 +4784,7 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>256</v>
       </c>
@@ -4782,7 +4797,7 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>258</v>
       </c>
@@ -4795,7 +4810,7 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>260</v>
       </c>
@@ -4808,7 +4823,7 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>262</v>
       </c>
@@ -4821,7 +4836,7 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>264</v>
       </c>
@@ -4834,7 +4849,7 @@
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>266</v>
       </c>
@@ -4847,7 +4862,7 @@
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>268</v>
       </c>
@@ -4860,7 +4875,7 @@
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>270</v>
       </c>
@@ -4873,7 +4888,7 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>272</v>
       </c>
@@ -4886,7 +4901,7 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>274</v>
       </c>
@@ -4899,7 +4914,7 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>276</v>
       </c>
@@ -4912,7 +4927,7 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -4930,13 +4945,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539D0DAF-3B47-4A29-A75D-3D6ADB320449}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -4956,7 +4971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4976,7 +4991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>646</v>
       </c>
@@ -4984,7 +4999,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>648</v>
       </c>
@@ -4992,7 +5007,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>649</v>
       </c>
@@ -5000,7 +5015,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>650</v>
       </c>
@@ -5008,7 +5023,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>651</v>
       </c>
@@ -5016,7 +5031,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>653</v>
       </c>
@@ -5034,12 +5049,12 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:F5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5059,7 +5074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>679</v>
       </c>
@@ -5067,7 +5082,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>681</v>
       </c>
@@ -5075,7 +5090,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>683</v>
       </c>
@@ -5083,7 +5098,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>685</v>
       </c>
@@ -5091,7 +5106,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>687</v>
       </c>
@@ -5099,7 +5114,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>689</v>
       </c>
@@ -5107,7 +5122,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>691</v>
       </c>
@@ -5128,9 +5143,9 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5150,7 +5165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>695</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>696</v>
       </c>
@@ -5180,9 +5195,9 @@
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5202,7 +5217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>699</v>
       </c>
@@ -5213,7 +5228,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>700</v>
       </c>
@@ -5224,7 +5239,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>701</v>
       </c>
@@ -5235,7 +5250,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>702</v>
       </c>
@@ -5260,14 +5275,14 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -5287,7 +5302,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5307,7 +5322,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>804</v>
       </c>
@@ -5321,7 +5336,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>805</v>
       </c>
@@ -5335,7 +5350,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>806</v>
       </c>
@@ -5349,7 +5364,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>807</v>
       </c>
@@ -5363,7 +5378,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>808</v>
       </c>
@@ -5377,7 +5392,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>809</v>
       </c>
@@ -5391,7 +5406,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>810</v>
       </c>
@@ -5405,7 +5420,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>811</v>
       </c>
@@ -5419,7 +5434,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>812</v>
       </c>
@@ -5433,7 +5448,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>813</v>
       </c>
@@ -5447,7 +5462,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>814</v>
       </c>
@@ -5461,7 +5476,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>815</v>
       </c>
@@ -5475,7 +5490,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>816</v>
       </c>
@@ -5489,7 +5504,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>817</v>
       </c>
@@ -5503,7 +5518,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>818</v>
       </c>
@@ -5517,7 +5532,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>819</v>
       </c>
@@ -5531,7 +5546,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>820</v>
       </c>
@@ -5545,7 +5560,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>821</v>
       </c>
@@ -5559,7 +5574,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>822</v>
       </c>
@@ -5573,7 +5588,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>823</v>
       </c>
@@ -5597,16 +5612,16 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -5626,7 +5641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5646,7 +5661,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>854</v>
       </c>
@@ -5660,7 +5675,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>855</v>
       </c>
@@ -5674,7 +5689,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>856</v>
       </c>
@@ -5688,7 +5703,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>857</v>
       </c>
@@ -5702,7 +5717,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>858</v>
       </c>
@@ -5716,7 +5731,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>859</v>
       </c>
@@ -5730,7 +5745,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>860</v>
       </c>
@@ -5744,7 +5759,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>861</v>
       </c>
@@ -5758,7 +5773,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>862</v>
       </c>
@@ -5772,7 +5787,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>863</v>
       </c>
@@ -5791,6 +5806,99 @@
     <hyperlink ref="F3" r:id="rId1" xr:uid="{1F779799-C8B2-499C-B7ED-E33915A311AB}"/>
     <hyperlink ref="F12" r:id="rId2" xr:uid="{C28B5BEF-4771-4915-BA25-24C55EFF2E13}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A254189-A980-43BE-BE8F-0FFFAFD05AA6}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>867</v>
+      </c>
+      <c r="B3" t="s">
+        <v>871</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>868</v>
+      </c>
+      <c r="B4" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>869</v>
+      </c>
+      <c r="B5" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>870</v>
+      </c>
+      <c r="B6" t="s">
+        <v>874</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5803,13 +5911,13 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -5829,7 +5937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5849,7 +5957,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>278</v>
       </c>
@@ -5860,7 +5968,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>280</v>
       </c>
@@ -5871,7 +5979,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>282</v>
       </c>
@@ -5882,7 +5990,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>284</v>
       </c>
@@ -5893,7 +6001,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>286</v>
       </c>
@@ -5904,7 +6012,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>288</v>
       </c>
@@ -5915,7 +6023,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>290</v>
       </c>
@@ -5935,7 +6043,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>295</v>
       </c>
@@ -5946,7 +6054,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>297</v>
       </c>
@@ -5957,7 +6065,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -5968,7 +6076,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>301</v>
       </c>
@@ -5979,7 +6087,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>303</v>
       </c>
@@ -5990,7 +6098,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>305</v>
       </c>
@@ -6001,7 +6109,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>307</v>
       </c>
@@ -6012,7 +6120,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>309</v>
       </c>
@@ -6023,7 +6131,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>311</v>
       </c>
@@ -6034,7 +6142,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>313</v>
       </c>
@@ -6045,7 +6153,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>315</v>
       </c>
@@ -6056,7 +6164,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>317</v>
       </c>
@@ -6067,7 +6175,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>319</v>
       </c>
@@ -6078,7 +6186,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>321</v>
       </c>
@@ -6089,7 +6197,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>323</v>
       </c>
@@ -6100,7 +6208,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>325</v>
       </c>
@@ -6111,7 +6219,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>327</v>
       </c>
@@ -6122,7 +6230,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>329</v>
       </c>
@@ -6133,7 +6241,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>331</v>
       </c>
@@ -6141,7 +6249,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>333</v>
       </c>
@@ -6149,7 +6257,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>335</v>
       </c>
@@ -6157,7 +6265,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>337</v>
       </c>
@@ -6165,7 +6273,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>339</v>
       </c>
@@ -6186,16 +6294,16 @@
       <selection activeCell="A2" sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -6215,7 +6323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6235,7 +6343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>341</v>
       </c>
@@ -6244,7 +6352,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>343</v>
       </c>
@@ -6252,7 +6360,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>345</v>
       </c>
@@ -6260,7 +6368,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>347</v>
       </c>
@@ -6268,7 +6376,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>349</v>
       </c>
@@ -6276,7 +6384,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>351</v>
       </c>
@@ -6284,7 +6392,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>353</v>
       </c>
@@ -6292,7 +6400,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>355</v>
       </c>
@@ -6300,7 +6408,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>357</v>
       </c>
@@ -6308,7 +6416,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>359</v>
       </c>
@@ -6316,7 +6424,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>361</v>
       </c>
@@ -6324,7 +6432,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>363</v>
       </c>
@@ -6332,7 +6440,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>365</v>
       </c>
@@ -6340,7 +6448,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>367</v>
       </c>
@@ -6348,7 +6456,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>369</v>
       </c>
@@ -6356,7 +6464,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>371</v>
       </c>
@@ -6364,7 +6472,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>373</v>
       </c>
@@ -6372,7 +6480,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>375</v>
       </c>
@@ -6380,7 +6488,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>377</v>
       </c>
@@ -6388,7 +6496,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>379</v>
       </c>
@@ -6396,7 +6504,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>381</v>
       </c>
@@ -6404,7 +6512,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>383</v>
       </c>
@@ -6412,7 +6520,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>385</v>
       </c>
@@ -6420,7 +6528,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>387</v>
       </c>
@@ -6428,7 +6536,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>389</v>
       </c>
@@ -6436,7 +6544,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>391</v>
       </c>
@@ -6444,7 +6552,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>393</v>
       </c>
@@ -6452,7 +6560,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>395</v>
       </c>
@@ -6460,7 +6568,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>397</v>
       </c>
@@ -6468,7 +6576,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>399</v>
       </c>
@@ -6476,7 +6584,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>401</v>
       </c>
@@ -6497,13 +6605,13 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -6523,7 +6631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6543,7 +6651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>403</v>
       </c>
@@ -6551,7 +6659,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>405</v>
       </c>
@@ -6559,7 +6667,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>407</v>
       </c>
@@ -6567,7 +6675,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>409</v>
       </c>
@@ -6575,7 +6683,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>411</v>
       </c>
@@ -6583,7 +6691,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -6591,7 +6699,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>415</v>
       </c>
@@ -6599,7 +6707,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>417</v>
       </c>
@@ -6607,7 +6715,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>419</v>
       </c>
@@ -6615,7 +6723,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>421</v>
       </c>
@@ -6623,7 +6731,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>423</v>
       </c>
@@ -6631,7 +6739,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>425</v>
       </c>
@@ -6639,7 +6747,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>427</v>
       </c>
@@ -6647,7 +6755,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>429</v>
       </c>
@@ -6655,7 +6763,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>431</v>
       </c>
@@ -6663,7 +6771,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>433</v>
       </c>
@@ -6671,7 +6779,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>435</v>
       </c>
@@ -6679,7 +6787,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>437</v>
       </c>
@@ -6687,7 +6795,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>439</v>
       </c>
@@ -6695,7 +6803,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>441</v>
       </c>
@@ -6703,7 +6811,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>443</v>
       </c>
@@ -6711,7 +6819,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>445</v>
       </c>
@@ -6719,7 +6827,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>447</v>
       </c>
@@ -6727,7 +6835,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>449</v>
       </c>
@@ -6735,7 +6843,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>451</v>
       </c>
@@ -6743,7 +6851,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>453</v>
       </c>
@@ -6751,7 +6859,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>455</v>
       </c>
@@ -6759,7 +6867,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>457</v>
       </c>
@@ -6767,7 +6875,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>459</v>
       </c>
@@ -6775,7 +6883,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>461</v>
       </c>
@@ -6783,7 +6891,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>463</v>
       </c>
@@ -6791,7 +6899,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>465</v>
       </c>
@@ -6799,7 +6907,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>467</v>
       </c>
@@ -6807,7 +6915,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>469</v>
       </c>
@@ -6815,7 +6923,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>471</v>
       </c>
@@ -6823,7 +6931,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>473</v>
       </c>
@@ -6831,7 +6939,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>475</v>
       </c>
@@ -6839,7 +6947,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>477</v>
       </c>
@@ -6860,14 +6968,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="59.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -6887,7 +6995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6907,7 +7015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>721</v>
       </c>
@@ -6918,7 +7026,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>722</v>
       </c>
@@ -6929,7 +7037,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>740</v>
       </c>
@@ -6940,7 +7048,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>723</v>
       </c>
@@ -6951,7 +7059,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>724</v>
       </c>
@@ -6962,7 +7070,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>725</v>
       </c>
@@ -6973,7 +7081,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>726</v>
       </c>
@@ -6984,7 +7092,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>727</v>
       </c>
@@ -6995,7 +7103,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>728</v>
       </c>
@@ -7006,7 +7114,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>729</v>
       </c>
@@ -7017,7 +7125,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>730</v>
       </c>
@@ -7028,7 +7136,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>731</v>
       </c>
@@ -7039,7 +7147,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>732</v>
       </c>
@@ -7050,7 +7158,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>733</v>
       </c>
@@ -7061,7 +7169,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>734</v>
       </c>
@@ -7072,7 +7180,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>735</v>
       </c>
@@ -7083,7 +7191,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>736</v>
       </c>
@@ -7094,7 +7202,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>737</v>
       </c>
@@ -7105,7 +7213,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>484</v>
       </c>
@@ -7116,7 +7224,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>738</v>
       </c>
@@ -7127,16 +7235,16 @@
         <v>742</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="9"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C25" s="9"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C26" s="9"/>
     </row>
   </sheetData>
@@ -7152,9 +7260,9 @@
       <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -7174,7 +7282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7194,7 +7302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>485</v>
       </c>
@@ -7202,7 +7310,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>487</v>
       </c>
@@ -7210,7 +7318,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>489</v>
       </c>
@@ -7219,7 +7327,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>491</v>
       </c>
@@ -7240,12 +7348,12 @@
       <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -7265,7 +7373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7285,7 +7393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>493</v>
       </c>
@@ -7296,7 +7404,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>496</v>
       </c>
@@ -7307,7 +7415,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>499</v>
       </c>
@@ -7327,17 +7435,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4C0B3A-7FCD-4BED-A793-C85D90A184F8}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -7357,7 +7465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7380,7 +7488,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>503</v>
       </c>
@@ -7388,7 +7496,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>505</v>
       </c>
@@ -7396,7 +7504,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>507</v>
       </c>
@@ -7404,7 +7512,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>509</v>
       </c>
@@ -7412,7 +7520,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>511</v>
       </c>
@@ -7420,7 +7528,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>513</v>
       </c>
@@ -7428,7 +7536,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>515</v>
       </c>
@@ -7436,7 +7544,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>517</v>
       </c>
@@ -7444,7 +7552,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>519</v>
       </c>
@@ -7452,7 +7560,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>521</v>
       </c>
@@ -7460,7 +7568,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>523</v>
       </c>
@@ -7468,7 +7576,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>525</v>
       </c>
@@ -7476,7 +7584,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>527</v>
       </c>
@@ -7484,7 +7592,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>529</v>
       </c>
@@ -7492,7 +7600,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>531</v>
       </c>
@@ -7500,7 +7608,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>533</v>
       </c>
@@ -7508,7 +7616,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>535</v>
       </c>
@@ -7516,7 +7624,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>537</v>
       </c>
@@ -7524,7 +7632,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>539</v>
       </c>
@@ -7532,7 +7640,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>541</v>
       </c>
@@ -7540,7 +7648,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>543</v>
       </c>
@@ -7548,7 +7656,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>545</v>
       </c>
@@ -7556,7 +7664,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>547</v>
       </c>
@@ -7564,7 +7672,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>549</v>
       </c>
@@ -7572,7 +7680,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>551</v>
       </c>
@@ -7580,7 +7688,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>553</v>
       </c>
@@ -7588,7 +7696,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>555</v>
       </c>
@@ -7596,7 +7704,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>557</v>
       </c>
@@ -7604,7 +7712,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>559</v>
       </c>
@@ -7612,7 +7720,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>561</v>
       </c>
@@ -7620,7 +7728,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>563</v>
       </c>
@@ -7628,7 +7736,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>565</v>
       </c>
@@ -7636,7 +7744,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>567</v>
       </c>
@@ -7644,7 +7752,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>569</v>
       </c>
@@ -7652,7 +7760,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>571</v>
       </c>
@@ -7660,7 +7768,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>573</v>
       </c>
@@ -7668,7 +7776,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>575</v>
       </c>
@@ -7676,7 +7784,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>577</v>
       </c>
@@ -7684,7 +7792,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>579</v>
       </c>
@@ -7692,7 +7800,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>581</v>
       </c>
@@ -7700,7 +7808,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>583</v>
       </c>
@@ -7708,7 +7816,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>585</v>
       </c>
@@ -7716,7 +7824,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>587</v>
       </c>
@@ -7724,7 +7832,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>589</v>
       </c>
@@ -7732,7 +7840,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>591</v>
       </c>
@@ -7740,7 +7848,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>593</v>
       </c>
@@ -7748,7 +7856,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>595</v>
       </c>
@@ -7756,7 +7864,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>597</v>
       </c>
@@ -7764,7 +7872,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>599</v>
       </c>
@@ -7772,7 +7880,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>601</v>
       </c>
@@ -7780,7 +7888,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>603</v>
       </c>
@@ -7788,7 +7896,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>605</v>
       </c>
@@ -7796,7 +7904,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>607</v>
       </c>
@@ -7804,7 +7912,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>609</v>
       </c>
@@ -7812,7 +7920,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>611</v>
       </c>
@@ -7820,7 +7928,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>613</v>
       </c>
@@ -7828,7 +7936,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>615</v>
       </c>
@@ -7836,7 +7944,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>617</v>
       </c>
@@ -7844,7 +7952,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>619</v>
       </c>
@@ -7852,7 +7960,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>621</v>
       </c>
@@ -7860,7 +7968,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>623</v>
       </c>
@@ -7868,7 +7976,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>625</v>
       </c>
@@ -7876,7 +7984,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>627</v>
       </c>
@@ -7884,7 +7992,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>629</v>
       </c>
@@ -7892,7 +8000,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>631</v>
       </c>
@@ -7900,7 +8008,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>633</v>
       </c>
@@ -7911,7 +8019,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>636</v>
       </c>
@@ -7935,12 +8043,12 @@
       <selection activeCell="J1" sqref="J1:J299"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -7960,7 +8068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -7980,7 +8088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>638</v>
       </c>
@@ -7988,7 +8096,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>640</v>
       </c>
@@ -7996,7 +8104,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>642</v>
       </c>
@@ -8004,7 +8112,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>644</v>
       </c>
@@ -8012,7 +8120,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>711</v>
       </c>

</xml_diff>

<commit_message>
ensure correct binary version
</commit_message>
<xml_diff>
--- a/xlsx/Lists.xlsx
+++ b/xlsx/Lists.xlsx
@@ -1,33 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="404" documentId="11_F25DC773A252ABDACC1048A6595D604E5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A227B620-8B34-4065-B621-0B50314FD73C}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{F75AE6B2-ADA3-4E57-BFA4-B07317854A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B17FFD97-A124-43E2-AEC3-A703546F09CB}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="15" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="01_Languages" sheetId="2" r:id="rId1"/>
-    <sheet name="02_Themes" sheetId="3" r:id="rId2"/>
-    <sheet name="03_Cultural Context" sheetId="4" r:id="rId3"/>
-    <sheet name="04_Social Groups" sheetId="5" r:id="rId4"/>
-    <sheet name="05_Rights" sheetId="6" r:id="rId5"/>
-    <sheet name="06_Gender" sheetId="7" r:id="rId6"/>
-    <sheet name="07_Cultural Sensitivity" sheetId="8" r:id="rId7"/>
-    <sheet name="08_Occupations" sheetId="9" r:id="rId8"/>
-    <sheet name="09_Project Types" sheetId="10" r:id="rId9"/>
-    <sheet name="10_Project Regions" sheetId="11" r:id="rId10"/>
-    <sheet name="11_Roles" sheetId="13" r:id="rId11"/>
-    <sheet name="12_Language Labels" sheetId="15" r:id="rId12"/>
-    <sheet name="13_Authority Sources" sheetId="16" r:id="rId13"/>
-    <sheet name="14_Traditional Knowledge Labels" sheetId="17" r:id="rId14"/>
-    <sheet name="15_Biocultural Labels" sheetId="18" r:id="rId15"/>
+    <sheet name="01_Languages (OBJ,ENT)" sheetId="2" r:id="rId1"/>
+    <sheet name="02_Keywords (OBJ)" sheetId="3" r:id="rId2"/>
+    <sheet name="03_Cultural Context (OBJ)" sheetId="4" r:id="rId3"/>
+    <sheet name="04_Social Groups (OBJ)" sheetId="5" r:id="rId4"/>
+    <sheet name="05_Rights (OBJ)" sheetId="6" r:id="rId5"/>
+    <sheet name="06_Gender (ENT)" sheetId="7" r:id="rId6"/>
+    <sheet name="07_Cultural Sensitivity (OBJ)" sheetId="8" r:id="rId7"/>
+    <sheet name="08_Occupations (ENT)" sheetId="9" r:id="rId8"/>
+    <sheet name="09_Project Types (COL)" sheetId="10" r:id="rId9"/>
+    <sheet name="10_Project Regions (COL)" sheetId="11" r:id="rId10"/>
+    <sheet name="11_Roles (ENT)" sheetId="13" r:id="rId11"/>
+    <sheet name="12_Resource Types (OBJ)" sheetId="20" r:id="rId12"/>
+    <sheet name="13_Authority Sources (ENT)" sheetId="16" r:id="rId13"/>
+    <sheet name="14_TraditionalKnowledge (OBJ)" sheetId="17" r:id="rId14"/>
+    <sheet name="15_Biocultural Labels (OBJ)" sheetId="18" r:id="rId15"/>
+    <sheet name="16_External Resources (PRJ)" sheetId="19" r:id="rId16"/>
+    <sheet name="17_Place Types (OBJ, COL, ENT)" sheetId="21" r:id="rId17"/>
+    <sheet name="18_Access Types (All)" sheetId="22" r:id="rId18"/>
+    <sheet name="19_Contributor Type (OBJ)" sheetId="23" r:id="rId19"/>
+    <sheet name="20_Publication Type (PRJ)" sheetId="24" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="1012">
   <si>
     <t>Term ID</t>
   </si>
@@ -1957,9 +1962,6 @@
     <t>Creators</t>
   </si>
   <si>
-    <t>newly added</t>
-  </si>
-  <si>
     <t>occupation_067</t>
   </si>
   <si>
@@ -1999,9 +2001,6 @@
     <t>reg_02</t>
   </si>
   <si>
-    <t>Asia Pasific</t>
-  </si>
-  <si>
     <t>reg_03</t>
   </si>
   <si>
@@ -2095,55 +2094,22 @@
     <t>role_01</t>
   </si>
   <si>
-    <t>Project leader</t>
-  </si>
-  <si>
     <t>role_02</t>
   </si>
   <si>
-    <t>Collector</t>
-  </si>
-  <si>
     <t>role_03</t>
   </si>
   <si>
-    <t>Monitor</t>
-  </si>
-  <si>
     <t>role_04</t>
   </si>
   <si>
-    <t>Contributor</t>
-  </si>
-  <si>
     <t>role_05</t>
   </si>
   <si>
-    <t>Administrator</t>
-  </si>
-  <si>
     <t>role_06</t>
   </si>
   <si>
-    <t>Guest</t>
-  </si>
-  <si>
     <t>role_07</t>
-  </si>
-  <si>
-    <t>Researcher</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>langlabel_01</t>
-  </si>
-  <si>
-    <t>langlabel_02</t>
   </si>
   <si>
     <t>VIAF</t>
@@ -2666,6 +2632,480 @@
   </si>
   <si>
     <t>GA_lang</t>
+  </si>
+  <si>
+    <t>Asia Pacific</t>
+  </si>
+  <si>
+    <t>exres_01</t>
+  </si>
+  <si>
+    <t>exres_02</t>
+  </si>
+  <si>
+    <t>exres_03</t>
+  </si>
+  <si>
+    <t>exres_04</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>Exhibition</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Interactive Form</t>
+  </si>
+  <si>
+    <t>prjtype_06</t>
+  </si>
+  <si>
+    <t>Further Initiatives (2023-2024)</t>
+  </si>
+  <si>
+    <t>role_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D Objects </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drawings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Film &amp; Media </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interview </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paintings </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photography </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prints </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recipe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sculptures </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Workshop </t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>drawing</t>
+  </si>
+  <si>
+    <t>film_media</t>
+  </si>
+  <si>
+    <t>interview</t>
+  </si>
+  <si>
+    <t>painting</t>
+  </si>
+  <si>
+    <t>performance</t>
+  </si>
+  <si>
+    <t>photography</t>
+  </si>
+  <si>
+    <t>print</t>
+  </si>
+  <si>
+    <t>recipe</t>
+  </si>
+  <si>
+    <t>sculpture</t>
+  </si>
+  <si>
+    <t>workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">countries </t>
+  </si>
+  <si>
+    <t xml:space="preserve">imaginary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">other features </t>
+  </si>
+  <si>
+    <t xml:space="preserve">regions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">town </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancentral non-geographical places </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Storytelling places </t>
+  </si>
+  <si>
+    <t xml:space="preserve">continents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">counties </t>
+  </si>
+  <si>
+    <t xml:space="preserve">locations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">neighborhoods </t>
+  </si>
+  <si>
+    <t xml:space="preserve">parishes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rivers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">state/province </t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>imaginary</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>town</t>
+  </si>
+  <si>
+    <t>imaginary_ancestral</t>
+  </si>
+  <si>
+    <t>imaginary_storytelling</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>neighborhood</t>
+  </si>
+  <si>
+    <t>socken</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accessible to public </t>
+  </si>
+  <si>
+    <t xml:space="preserve">not accessible to public </t>
+  </si>
+  <si>
+    <t xml:space="preserve">restricted public access </t>
+  </si>
+  <si>
+    <t>internal_only</t>
+  </si>
+  <si>
+    <t>restricted_public_access</t>
+  </si>
+  <si>
+    <t>public_access</t>
+  </si>
+  <si>
+    <t xml:space="preserve">staff member </t>
+  </si>
+  <si>
+    <t xml:space="preserve">architect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">artist </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has as author </t>
+  </si>
+  <si>
+    <t xml:space="preserve">curator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">consultant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">panelist </t>
+  </si>
+  <si>
+    <t xml:space="preserve">designer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentarian </t>
+  </si>
+  <si>
+    <t xml:space="preserve">publisher </t>
+  </si>
+  <si>
+    <t xml:space="preserve">moderator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">speaker </t>
+  </si>
+  <si>
+    <t xml:space="preserve">partner </t>
+  </si>
+  <si>
+    <t xml:space="preserve">performer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sponsor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinematography by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">creator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Directed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edition by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">interviewee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lightning by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music authors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music Mixed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music performed by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music produced by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music Rights </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music Rights Held </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Music titles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">photographer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produced by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rights holder </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sound by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Written by </t>
+  </si>
+  <si>
+    <t>staff_member</t>
+  </si>
+  <si>
+    <t>architect</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>curator</t>
+  </si>
+  <si>
+    <t>consultant</t>
+  </si>
+  <si>
+    <t>panelist</t>
+  </si>
+  <si>
+    <t>designer</t>
+  </si>
+  <si>
+    <t>documentarian</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>moderator</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>partner_museum</t>
+  </si>
+  <si>
+    <t>performer</t>
+  </si>
+  <si>
+    <t>sponsor</t>
+  </si>
+  <si>
+    <t>cinematography_by</t>
+  </si>
+  <si>
+    <t>contributor</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>directed_by</t>
+  </si>
+  <si>
+    <t>edition_by</t>
+  </si>
+  <si>
+    <t>interviewee</t>
+  </si>
+  <si>
+    <t>lightning_by</t>
+  </si>
+  <si>
+    <t>music_authors</t>
+  </si>
+  <si>
+    <t>music_mixed_by</t>
+  </si>
+  <si>
+    <t>music_performed_by</t>
+  </si>
+  <si>
+    <t>music_produced_by</t>
+  </si>
+  <si>
+    <t>music_rights</t>
+  </si>
+  <si>
+    <t>music_rights_held</t>
+  </si>
+  <si>
+    <t>music_titles</t>
+  </si>
+  <si>
+    <t>photographer</t>
+  </si>
+  <si>
+    <t>produced_by</t>
+  </si>
+  <si>
+    <t>rightsholder</t>
+  </si>
+  <si>
+    <t>sound_by</t>
+  </si>
+  <si>
+    <t>written_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrator </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advisors </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core Team </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fellows </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MA Fellows </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organisations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research Partners </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Support Team </t>
+  </si>
+  <si>
+    <t>Volume A</t>
+  </si>
+  <si>
+    <t>Volume B</t>
+  </si>
+  <si>
+    <t>vol_a</t>
+  </si>
+  <si>
+    <t>vol_b</t>
   </si>
 </sst>
 </file>
@@ -2809,10 +3249,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3078,18 +3514,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C7DCC5-93A4-4F15-9716-2215F2C5540F}">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -3110,7 +3550,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3131,7 +3571,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -3144,7 +3584,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3157,7 +3597,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -3170,7 +3610,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -3183,7 +3623,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -3196,7 +3636,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -3209,7 +3649,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -3222,7 +3662,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -3235,7 +3675,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -3248,7 +3688,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -3261,7 +3701,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -3272,9 +3712,8 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -3285,9 +3724,9 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -3298,9 +3737,8 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3310,8 +3748,6 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
@@ -3324,7 +3760,6 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -3337,7 +3772,6 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -3350,7 +3784,6 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -3363,7 +3796,6 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -3376,7 +3808,6 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -3389,7 +3820,6 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3614,10 +4044,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>866</v>
+        <v>853</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>865</v>
+        <v>852</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -4931,7 +5361,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,50 +5408,50 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>645</v>
+      </c>
+      <c r="B3" t="s">
         <v>646</v>
-      </c>
-      <c r="B3" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B4" t="s">
-        <v>649</v>
+        <v>854</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B5" t="s">
-        <v>710</v>
+        <v>697</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B6" t="s">
-        <v>711</v>
+        <v>698</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B7" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="B8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -5031,10 +5461,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F350B9F1-06F7-4E8A-B44A-16E139FB0B1D}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:F5"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5061,74 +5491,91 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B2" t="s">
-        <v>681</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="B3" t="s">
-        <v>683</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B4" t="s">
-        <v>685</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="B5" t="s">
-        <v>687</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>688</v>
+        <v>682</v>
       </c>
       <c r="B6" t="s">
-        <v>689</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="B7" t="s">
-        <v>691</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="B8" t="s">
-        <v>693</v>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>865</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1007</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
+    <sortCondition ref="A1:A9"/>
+  </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5D6CC2-7C88-44F7-8C63-8AD47A42CD2B}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07921A81-EB7F-4120-B1F0-4C6362E633AA}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -5152,22 +5599,117 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>696</v>
+        <v>880</v>
       </c>
       <c r="B2" t="s">
-        <v>694</v>
+        <v>866</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>697</v>
+        <v>881</v>
       </c>
       <c r="B3" t="s">
-        <v>695</v>
+        <v>867</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>882</v>
+      </c>
+      <c r="B4" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>883</v>
+      </c>
+      <c r="B5" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>884</v>
+      </c>
+      <c r="B6" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B7" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>886</v>
+      </c>
+      <c r="B8" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>887</v>
+      </c>
+      <c r="B9" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>888</v>
+      </c>
+      <c r="B10" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>889</v>
+      </c>
+      <c r="B11" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>890</v>
+      </c>
+      <c r="B12" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>891</v>
+      </c>
+      <c r="B13" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>892</v>
+      </c>
+      <c r="B14" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>893</v>
+      </c>
+      <c r="B15" t="s">
+        <v>879</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5204,46 +5746,46 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="B2" t="s">
-        <v>698</v>
+        <v>685</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>706</v>
+        <v>693</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="B3" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>709</v>
+        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>702</v>
+        <v>689</v>
       </c>
       <c r="B4" t="s">
-        <v>704</v>
+        <v>691</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>707</v>
+        <v>694</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>703</v>
+        <v>690</v>
       </c>
       <c r="B5" t="s">
-        <v>705</v>
+        <v>692</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>708</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -5257,7 +5799,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5304,287 +5846,287 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>805</v>
+        <v>792</v>
       </c>
       <c r="B3" t="s">
-        <v>744</v>
+        <v>731</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>745</v>
+        <v>732</v>
       </c>
       <c r="F3" t="s">
-        <v>746</v>
+        <v>733</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>806</v>
+        <v>793</v>
       </c>
       <c r="B4" t="s">
-        <v>747</v>
+        <v>734</v>
       </c>
       <c r="C4" t="s">
-        <v>748</v>
+        <v>735</v>
       </c>
       <c r="F4" t="s">
-        <v>749</v>
+        <v>736</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>807</v>
+        <v>794</v>
       </c>
       <c r="B5" t="s">
-        <v>750</v>
+        <v>737</v>
       </c>
       <c r="C5" t="s">
-        <v>751</v>
+        <v>738</v>
       </c>
       <c r="F5" t="s">
-        <v>755</v>
+        <v>742</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>808</v>
+        <v>795</v>
       </c>
       <c r="B6" t="s">
-        <v>752</v>
+        <v>739</v>
       </c>
       <c r="C6" t="s">
-        <v>753</v>
+        <v>740</v>
       </c>
       <c r="F6" t="s">
-        <v>754</v>
+        <v>741</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>809</v>
+        <v>796</v>
       </c>
       <c r="B7" t="s">
-        <v>756</v>
+        <v>743</v>
       </c>
       <c r="C7" t="s">
-        <v>757</v>
+        <v>744</v>
       </c>
       <c r="F7" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>810</v>
+        <v>797</v>
       </c>
       <c r="B8" t="s">
-        <v>759</v>
+        <v>746</v>
       </c>
       <c r="C8" t="s">
-        <v>760</v>
+        <v>747</v>
       </c>
       <c r="F8" t="s">
-        <v>761</v>
+        <v>748</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>811</v>
+        <v>798</v>
       </c>
       <c r="B9" t="s">
-        <v>762</v>
+        <v>749</v>
       </c>
       <c r="C9" t="s">
-        <v>763</v>
+        <v>750</v>
       </c>
       <c r="F9" t="s">
-        <v>764</v>
+        <v>751</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>812</v>
+        <v>799</v>
       </c>
       <c r="B10" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="C10" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="F10" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>813</v>
+        <v>800</v>
       </c>
       <c r="B11" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="C11" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="F11" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="B12" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="C12" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="F12" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="B13" t="s">
-        <v>774</v>
+        <v>761</v>
       </c>
       <c r="C13" t="s">
-        <v>775</v>
+        <v>762</v>
       </c>
       <c r="F13" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="B14" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
       <c r="C14" t="s">
-        <v>779</v>
+        <v>766</v>
       </c>
       <c r="F14" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>817</v>
+        <v>804</v>
       </c>
       <c r="B15" t="s">
-        <v>781</v>
+        <v>768</v>
       </c>
       <c r="C15" t="s">
-        <v>782</v>
+        <v>769</v>
       </c>
       <c r="F15" t="s">
-        <v>780</v>
+        <v>767</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>818</v>
+        <v>805</v>
       </c>
       <c r="B16" t="s">
-        <v>783</v>
+        <v>770</v>
       </c>
       <c r="C16" t="s">
-        <v>785</v>
+        <v>772</v>
       </c>
       <c r="F16" t="s">
-        <v>784</v>
+        <v>771</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>819</v>
+        <v>806</v>
       </c>
       <c r="B17" t="s">
-        <v>786</v>
+        <v>773</v>
       </c>
       <c r="C17" t="s">
-        <v>787</v>
+        <v>774</v>
       </c>
       <c r="F17" t="s">
-        <v>788</v>
+        <v>775</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>820</v>
+        <v>807</v>
       </c>
       <c r="B18" t="s">
-        <v>789</v>
+        <v>776</v>
       </c>
       <c r="C18" t="s">
-        <v>791</v>
+        <v>778</v>
       </c>
       <c r="F18" t="s">
-        <v>790</v>
+        <v>777</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>821</v>
+        <v>808</v>
       </c>
       <c r="B19" t="s">
-        <v>792</v>
+        <v>779</v>
       </c>
       <c r="C19" t="s">
-        <v>793</v>
+        <v>780</v>
       </c>
       <c r="F19" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>822</v>
+        <v>809</v>
       </c>
       <c r="B20" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="C20" t="s">
-        <v>796</v>
+        <v>783</v>
       </c>
       <c r="F20" t="s">
-        <v>797</v>
+        <v>784</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>823</v>
+        <v>810</v>
       </c>
       <c r="B21" t="s">
-        <v>798</v>
+        <v>785</v>
       </c>
       <c r="C21" t="s">
-        <v>799</v>
+        <v>786</v>
       </c>
       <c r="F21" t="s">
-        <v>800</v>
+        <v>787</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>824</v>
+        <v>811</v>
       </c>
       <c r="B22" t="s">
-        <v>801</v>
+        <v>788</v>
       </c>
       <c r="C22" t="s">
-        <v>802</v>
+        <v>789</v>
       </c>
       <c r="F22" t="s">
-        <v>803</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>
@@ -5597,7 +6139,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5643,147 +6185,147 @@
         <v>4</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>804</v>
+        <v>791</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>855</v>
+        <v>842</v>
       </c>
       <c r="B3" t="s">
-        <v>825</v>
+        <v>812</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>826</v>
+        <v>813</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>827</v>
+        <v>814</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>856</v>
+        <v>843</v>
       </c>
       <c r="B4" t="s">
-        <v>829</v>
+        <v>816</v>
       </c>
       <c r="C4" t="s">
-        <v>830</v>
+        <v>817</v>
       </c>
       <c r="F4" t="s">
-        <v>828</v>
+        <v>815</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>857</v>
+        <v>844</v>
       </c>
       <c r="B5" t="s">
-        <v>832</v>
+        <v>819</v>
       </c>
       <c r="C5" t="s">
-        <v>833</v>
+        <v>820</v>
       </c>
       <c r="F5" t="s">
-        <v>831</v>
+        <v>818</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>858</v>
+        <v>845</v>
       </c>
       <c r="B6" t="s">
-        <v>835</v>
+        <v>822</v>
       </c>
       <c r="C6" t="s">
-        <v>836</v>
+        <v>823</v>
       </c>
       <c r="F6" t="s">
-        <v>834</v>
+        <v>821</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>859</v>
+        <v>846</v>
       </c>
       <c r="B7" t="s">
-        <v>837</v>
+        <v>824</v>
       </c>
       <c r="C7" t="s">
-        <v>838</v>
+        <v>825</v>
       </c>
       <c r="F7" t="s">
-        <v>839</v>
+        <v>826</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>860</v>
+        <v>847</v>
       </c>
       <c r="B8" t="s">
-        <v>842</v>
+        <v>829</v>
       </c>
       <c r="C8" t="s">
-        <v>841</v>
+        <v>828</v>
       </c>
       <c r="F8" t="s">
-        <v>840</v>
+        <v>827</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>861</v>
+        <v>848</v>
       </c>
       <c r="B9" t="s">
-        <v>845</v>
+        <v>832</v>
       </c>
       <c r="C9" t="s">
-        <v>843</v>
+        <v>830</v>
       </c>
       <c r="F9" t="s">
-        <v>844</v>
+        <v>831</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>862</v>
+        <v>849</v>
       </c>
       <c r="B10" t="s">
-        <v>846</v>
+        <v>833</v>
       </c>
       <c r="C10" t="s">
-        <v>847</v>
+        <v>834</v>
       </c>
       <c r="F10" t="s">
-        <v>848</v>
+        <v>835</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>863</v>
+        <v>850</v>
       </c>
       <c r="B11" t="s">
-        <v>849</v>
+        <v>836</v>
       </c>
       <c r="C11" t="s">
-        <v>850</v>
+        <v>837</v>
       </c>
       <c r="F11" t="s">
-        <v>851</v>
+        <v>838</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>864</v>
+        <v>851</v>
       </c>
       <c r="B12" t="s">
-        <v>853</v>
+        <v>840</v>
       </c>
       <c r="C12" t="s">
-        <v>854</v>
+        <v>841</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>852</v>
+        <v>839</v>
       </c>
     </row>
   </sheetData>
@@ -5795,12 +6337,701 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A254189-A980-43BE-BE8F-0FFFAFD05AA6}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>855</v>
+      </c>
+      <c r="B3" t="s">
+        <v>859</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>856</v>
+      </c>
+      <c r="B4" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>857</v>
+      </c>
+      <c r="B5" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>858</v>
+      </c>
+      <c r="B6" t="s">
+        <v>862</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3AD6D0-A39E-40B0-AC16-D83F3095D822}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>910</v>
+      </c>
+      <c r="B3" t="s">
+        <v>894</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>911</v>
+      </c>
+      <c r="B4" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>925</v>
+      </c>
+      <c r="B5" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>912</v>
+      </c>
+      <c r="B6" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>913</v>
+      </c>
+      <c r="B7" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>914</v>
+      </c>
+      <c r="B8" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>915</v>
+      </c>
+      <c r="B9" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>916</v>
+      </c>
+      <c r="B10" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>917</v>
+      </c>
+      <c r="B11" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>918</v>
+      </c>
+      <c r="B12" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>919</v>
+      </c>
+      <c r="B13" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>920</v>
+      </c>
+      <c r="B14" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>921</v>
+      </c>
+      <c r="B15" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>922</v>
+      </c>
+      <c r="B16" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>923</v>
+      </c>
+      <c r="B17" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>924</v>
+      </c>
+      <c r="B18" t="s">
+        <v>909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68688104-DADE-48DC-AAF4-708FF27F4233}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>931</v>
+      </c>
+      <c r="B3" t="s">
+        <v>926</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>929</v>
+      </c>
+      <c r="B4" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>930</v>
+      </c>
+      <c r="B5" t="s">
+        <v>928</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6FB8C1-8B47-4222-8F27-60EA6C8E341E}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B3" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>967</v>
+      </c>
+      <c r="B4" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>968</v>
+      </c>
+      <c r="B5" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>969</v>
+      </c>
+      <c r="B6" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>970</v>
+      </c>
+      <c r="B7" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>971</v>
+      </c>
+      <c r="B8" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>972</v>
+      </c>
+      <c r="B9" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>973</v>
+      </c>
+      <c r="B10" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>974</v>
+      </c>
+      <c r="B11" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>975</v>
+      </c>
+      <c r="B12" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>976</v>
+      </c>
+      <c r="B13" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>977</v>
+      </c>
+      <c r="B14" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>978</v>
+      </c>
+      <c r="B15" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>979</v>
+      </c>
+      <c r="B16" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>980</v>
+      </c>
+      <c r="B17" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>981</v>
+      </c>
+      <c r="B18" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>982</v>
+      </c>
+      <c r="B19" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>983</v>
+      </c>
+      <c r="B20" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>984</v>
+      </c>
+      <c r="B21" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>985</v>
+      </c>
+      <c r="B22" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>986</v>
+      </c>
+      <c r="B23" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>987</v>
+      </c>
+      <c r="B24" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>988</v>
+      </c>
+      <c r="B25" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>989</v>
+      </c>
+      <c r="B26" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>990</v>
+      </c>
+      <c r="B27" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>991</v>
+      </c>
+      <c r="B28" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>992</v>
+      </c>
+      <c r="B29" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>993</v>
+      </c>
+      <c r="B30" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>994</v>
+      </c>
+      <c r="B31" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>995</v>
+      </c>
+      <c r="B32" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>996</v>
+      </c>
+      <c r="B33" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>997</v>
+      </c>
+      <c r="B34" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>998</v>
+      </c>
+      <c r="B35" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>999</v>
+      </c>
+      <c r="B36" t="s">
+        <v>965</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477AB8E0-193B-4ACE-9281-1EB5DE711D3C}">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6171,6 +7402,77 @@
       </c>
       <c r="B32" s="1" t="s">
         <v>340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8BC3D3-1126-46C1-92F7-8E99091725FF}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1009</v>
       </c>
     </row>
   </sheetData>
@@ -6494,7 +7796,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6856,7 +8158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B29326D-C093-4910-A1C0-5F486B1575C8}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -6909,10 +8211,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>722</v>
+        <v>709</v>
       </c>
       <c r="B3" t="s">
-        <v>714</v>
+        <v>701</v>
       </c>
       <c r="C3" t="s">
         <v>479</v>
@@ -6920,21 +8222,21 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>723</v>
+        <v>710</v>
       </c>
       <c r="B4" t="s">
-        <v>715</v>
+        <v>702</v>
       </c>
       <c r="C4" t="s">
-        <v>740</v>
+        <v>727</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>741</v>
+        <v>728</v>
       </c>
       <c r="B5" t="s">
-        <v>716</v>
+        <v>703</v>
       </c>
       <c r="C5" t="s">
         <v>483</v>
@@ -6942,10 +8244,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>724</v>
+        <v>711</v>
       </c>
       <c r="B6" t="s">
-        <v>717</v>
+        <v>704</v>
       </c>
       <c r="C6" t="s">
         <v>482</v>
@@ -6953,10 +8255,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>725</v>
+        <v>712</v>
       </c>
       <c r="B7" t="s">
-        <v>718</v>
+        <v>705</v>
       </c>
       <c r="C7" t="s">
         <v>481</v>
@@ -6964,10 +8266,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>726</v>
+        <v>713</v>
       </c>
       <c r="B8" t="s">
-        <v>719</v>
+        <v>706</v>
       </c>
       <c r="C8" t="s">
         <v>480</v>
@@ -6975,134 +8277,134 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>727</v>
+        <v>714</v>
       </c>
       <c r="B9" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C9" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>728</v>
+        <v>715</v>
       </c>
       <c r="B10" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="C10" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>729</v>
+        <v>716</v>
       </c>
       <c r="B11" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="C11" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>730</v>
+        <v>717</v>
       </c>
       <c r="B12" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C12" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>731</v>
+        <v>718</v>
       </c>
       <c r="B13" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="C13" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>732</v>
+        <v>719</v>
       </c>
       <c r="B14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="C14" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
       <c r="B15" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C15" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>734</v>
+        <v>721</v>
       </c>
       <c r="B16" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="C16" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>735</v>
+        <v>722</v>
       </c>
       <c r="B17" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="C17" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>736</v>
+        <v>723</v>
       </c>
       <c r="B18" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="C18" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>737</v>
+        <v>724</v>
       </c>
       <c r="B19" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="C19" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>738</v>
+        <v>725</v>
       </c>
       <c r="B20" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="C20" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -7110,21 +8412,21 @@
         <v>484</v>
       </c>
       <c r="B21" t="s">
-        <v>720</v>
+        <v>707</v>
       </c>
       <c r="C21" t="s">
-        <v>742</v>
+        <v>729</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>739</v>
+        <v>726</v>
       </c>
       <c r="B22" t="s">
-        <v>721</v>
+        <v>708</v>
       </c>
       <c r="C22" t="s">
-        <v>743</v>
+        <v>730</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -7149,7 +8451,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7327,8 +8629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA4C0B3A-7FCD-4BED-A793-C85D90A184F8}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7876,7 +9178,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>627</v>
       </c>
@@ -7884,7 +9186,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>629</v>
       </c>
@@ -7892,7 +9194,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>631</v>
       </c>
@@ -7900,26 +9202,20 @@
         <v>632</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>633</v>
       </c>
       <c r="B68" t="s">
         <v>634</v>
       </c>
-      <c r="C68" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B69" s="7" t="s">
         <v>636</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>637</v>
-      </c>
-      <c r="C69" t="s">
-        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -7929,10 +9225,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F08A626F-F860-4615-8CDE-0A8AB0EDDB54}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J299"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7982,42 +9278,50 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B3" t="s">
         <v>638</v>
-      </c>
-      <c r="B3" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>639</v>
+      </c>
+      <c r="B4" t="s">
         <v>640</v>
-      </c>
-      <c r="B4" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>641</v>
+      </c>
+      <c r="B5" t="s">
         <v>642</v>
-      </c>
-      <c r="B5" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>643</v>
+      </c>
+      <c r="B6" t="s">
         <v>644</v>
-      </c>
-      <c r="B6" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>712</v>
+        <v>699</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>713</v>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>863</v>
+      </c>
+      <c r="B8" t="s">
+        <v>864</v>
       </c>
     </row>
   </sheetData>

</xml_diff>